<commit_message>
Backbone excel statiek staat
</commit_message>
<xml_diff>
--- a/pract3/Gebruiksreview Body Photo Browser (Reacties).xlsx
+++ b/pract3/Gebruiksreview Body Photo Browser (Reacties).xlsx
@@ -13,14 +13,16 @@
   </bookViews>
   <sheets>
     <sheet name="Formulierreacties 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad1" sheetId="2" r:id="rId2"/>
+    <sheet name="PSSUQ" sheetId="2" r:id="rId2"/>
+    <sheet name="SEQ" sheetId="4" r:id="rId3"/>
+    <sheet name="ASQ" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>Tijdstempel</t>
   </si>
@@ -149,6 +151,114 @@
   </si>
   <si>
     <t>Scenario</t>
+  </si>
+  <si>
+    <t>sc1.1</t>
+  </si>
+  <si>
+    <t>sc1.2</t>
+  </si>
+  <si>
+    <t>sc1.3</t>
+  </si>
+  <si>
+    <t>sc2.1</t>
+  </si>
+  <si>
+    <t>sc2.2</t>
+  </si>
+  <si>
+    <t>sc2.3</t>
+  </si>
+  <si>
+    <t>sc3.1</t>
+  </si>
+  <si>
+    <t>sc3.2</t>
+  </si>
+  <si>
+    <t>sc3.3</t>
+  </si>
+  <si>
+    <t>sc4.1</t>
+  </si>
+  <si>
+    <t>sc4.2</t>
+  </si>
+  <si>
+    <t>sc4.3</t>
+  </si>
+  <si>
+    <t>sc5.1</t>
+  </si>
+  <si>
+    <t>sc5.2</t>
+  </si>
+  <si>
+    <t>sc5.3</t>
+  </si>
+  <si>
+    <t>sc6.1</t>
+  </si>
+  <si>
+    <t>sc6.2</t>
+  </si>
+  <si>
+    <t>sc6.3</t>
+  </si>
+  <si>
+    <t>sc7.1</t>
+  </si>
+  <si>
+    <t>sc7.2</t>
+  </si>
+  <si>
+    <t>sc7.3</t>
+  </si>
+  <si>
+    <t>sc8.1</t>
+  </si>
+  <si>
+    <t>sc8.2</t>
+  </si>
+  <si>
+    <t>sc8.3</t>
+  </si>
+  <si>
+    <t>sc9.1</t>
+  </si>
+  <si>
+    <t>sc9.2</t>
+  </si>
+  <si>
+    <t>sc9.3</t>
+  </si>
+  <si>
+    <t>sc10.1</t>
+  </si>
+  <si>
+    <t>sc10.2</t>
+  </si>
+  <si>
+    <t>sc10.3</t>
+  </si>
+  <si>
+    <t>reactie</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>stdev</t>
+  </si>
+  <si>
+    <t>skew</t>
+  </si>
+  <si>
+    <t>kurt</t>
+  </si>
+  <si>
+    <t>mean_scen</t>
   </si>
 </sst>
 </file>
@@ -194,7 +304,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -227,11 +337,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -240,6 +361,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1311,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J41" sqref="A30:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1365,7 +1491,7 @@
       </c>
       <c r="H2">
         <f xml:space="preserve"> I2 - ($M$3*G2/SQRT($M$1))</f>
-        <v>1.9544999999999999</v>
+        <v>1.9543884236790727</v>
       </c>
       <c r="I2">
         <f>AVERAGE(B2:E2)</f>
@@ -1373,12 +1499,13 @@
       </c>
       <c r="J2">
         <f xml:space="preserve"> I2 + ($M$3*G2/SQRT($M$1))</f>
-        <v>3.5455000000000001</v>
+        <v>3.545611576320927</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>35</v>
       </c>
       <c r="M2">
+        <f>M1-1</f>
         <v>3</v>
       </c>
     </row>
@@ -1399,26 +1526,27 @@
         <v>4</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G16" si="0">_xlfn.STDEV.S(B3:E3)</f>
+        <f>_xlfn.STDEV.S(B3:E3)</f>
         <v>0.9574271077563381</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H14" si="1" xml:space="preserve"> I3 - ($M$3*G3/SQRT($M$1))</f>
-        <v>1.2267334715596661</v>
+        <f xml:space="preserve"> I3 - ($M$3*G3/SQRT($M$1))</f>
+        <v>1.226519819171187</v>
       </c>
       <c r="I3">
         <f>AVERAGE(B3:E3)</f>
         <v>2.75</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J14" si="2" xml:space="preserve"> I3 + ($M$3*G3/SQRT($M$1))</f>
-        <v>4.2732665284403337</v>
+        <f xml:space="preserve"> I3 + ($M$3*G3/SQRT($M$1))</f>
+        <v>4.2734801808288125</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>36</v>
       </c>
       <c r="M3">
-        <v>3.1819999999999999</v>
+        <f>_xlfn.T.INV.2T(0.05, M2)</f>
+        <v>3.1824463052837091</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1438,20 +1566,20 @@
         <v>3</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B4:E4)</f>
         <v>0.5</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>1.9544999999999999</v>
+        <f xml:space="preserve"> I4 - ($M$3*G4/SQRT($M$1))</f>
+        <v>1.9543884236790727</v>
       </c>
       <c r="I4">
         <f>AVERAGE(B4:E4)</f>
         <v>2.75</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
-        <v>3.5455000000000001</v>
+        <f xml:space="preserve"> I4 + ($M$3*G4/SQRT($M$1))</f>
+        <v>3.545611576320927</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1471,20 +1599,20 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B5:E5)</f>
         <v>1.4142135623730951</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>0.74998622226440581</v>
+        <f xml:space="preserve"> I5 - ($M$3*G5/SQRT($M$1))</f>
+        <v>0.74967063677181534</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I16" si="3">AVERAGE(B5:E5)</f>
+        <f>AVERAGE(B5:E5)</f>
         <v>3</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
-        <v>5.2500137777355942</v>
+        <f xml:space="preserve"> I5 + ($M$3*G5/SQRT($M$1))</f>
+        <v>5.2503293632281842</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1504,20 +1632,20 @@
         <v>4</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B6:E6)</f>
         <v>0.9574271077563381</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>1.2267334715596661</v>
+        <f xml:space="preserve"> I6 - ($M$3*G6/SQRT($M$1))</f>
+        <v>1.226519819171187</v>
       </c>
       <c r="I6">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(B6:E6)</f>
         <v>2.75</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
-        <v>4.2732665284403337</v>
+        <f xml:space="preserve"> I6 + ($M$3*G6/SQRT($M$1))</f>
+        <v>4.2734801808288125</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1537,20 +1665,20 @@
         <v>4</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B7:E7)</f>
         <v>0.9574271077563381</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>1.7267334715596661</v>
+        <f xml:space="preserve"> I7 - ($M$3*G7/SQRT($M$1))</f>
+        <v>1.726519819171187</v>
       </c>
       <c r="I7">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(B7:E7)</f>
         <v>3.25</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
-        <v>4.7732665284403337</v>
+        <f xml:space="preserve"> I7 + ($M$3*G7/SQRT($M$1))</f>
+        <v>4.7734801808288125</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1570,20 +1698,20 @@
         <v>7</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B8:E8)</f>
         <v>1.5</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>3.3635000000000002</v>
+        <f xml:space="preserve"> I8 - ($M$3*G8/SQRT($M$1))</f>
+        <v>3.363165271037218</v>
       </c>
       <c r="I8">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(B8:E8)</f>
         <v>5.75</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
-        <v>8.1364999999999998</v>
+        <f xml:space="preserve"> I8 + ($M$3*G8/SQRT($M$1))</f>
+        <v>8.136834728962782</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1603,20 +1731,20 @@
         <v>5</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B9:E9)</f>
         <v>0.81649658092772603</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
-        <v>2.7009539397439877</v>
+        <f xml:space="preserve"> I9 - ($M$3*G9/SQRT($M$1))</f>
+        <v>2.7007717363748887</v>
       </c>
       <c r="I9">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(B9:E9)</f>
         <v>4</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
-        <v>5.2990460602560123</v>
+        <f xml:space="preserve"> I9 + ($M$3*G9/SQRT($M$1))</f>
+        <v>5.2992282636251113</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1636,20 +1764,20 @@
         <v>4</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B10:E10)</f>
         <v>1.7320508075688772</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>1.7443071651579163</v>
+        <f xml:space="preserve"> I10 - ($M$3*G10/SQRT($M$1))</f>
+        <v>1.743920653444381</v>
       </c>
       <c r="I10">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(B10:E10)</f>
         <v>4.5</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
-        <v>7.2556928348420833</v>
+        <f xml:space="preserve"> I10 + ($M$3*G10/SQRT($M$1))</f>
+        <v>7.2560793465556195</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1669,20 +1797,20 @@
         <v>7</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B11:E11)</f>
         <v>1.4142135623730951</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>2.7499862222644058</v>
+        <f xml:space="preserve"> I11 - ($M$3*G11/SQRT($M$1))</f>
+        <v>2.7496706367718153</v>
       </c>
       <c r="I11">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(B11:E11)</f>
         <v>5</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
-        <v>7.2500137777355942</v>
+        <f xml:space="preserve"> I11 + ($M$3*G11/SQRT($M$1))</f>
+        <v>7.2503293632281842</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1702,20 +1830,20 @@
         <v>7</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B12:E12)</f>
         <v>1.5</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
-        <v>2.3635000000000002</v>
+        <f xml:space="preserve"> I12 - ($M$3*G12/SQRT($M$1))</f>
+        <v>2.363165271037218</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(B12:E12)</f>
         <v>4.75</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
-        <v>7.1364999999999998</v>
+        <f xml:space="preserve"> I12 + ($M$3*G12/SQRT($M$1))</f>
+        <v>7.136834728962782</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1735,20 +1863,20 @@
         <v>4</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B13:E13)</f>
         <v>1.4142135623730951</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
-        <v>2.7499862222644058</v>
+        <f xml:space="preserve"> I13 - ($M$3*G13/SQRT($M$1))</f>
+        <v>2.7496706367718153</v>
       </c>
       <c r="I13">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(B13:E13)</f>
         <v>5</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
-        <v>7.2500137777355942</v>
+        <f xml:space="preserve"> I13 + ($M$3*G13/SQRT($M$1))</f>
+        <v>7.2503293632281842</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1768,20 +1896,20 @@
         <v>4</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f>_xlfn.STDEV.S(B14:E14)</f>
         <v>1.4142135623730951</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
-        <v>0.74998622226440581</v>
+        <f xml:space="preserve"> I14 - ($M$3*G14/SQRT($M$1))</f>
+        <v>0.74967063677181534</v>
       </c>
       <c r="I14">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(B14:E14)</f>
         <v>3</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
-        <v>5.2500137777355942</v>
+        <f xml:space="preserve"> I14 + ($M$3*G14/SQRT($M$1))</f>
+        <v>5.2503293632281842</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1806,7 +1934,7 @@
       </c>
       <c r="H15">
         <f xml:space="preserve"> I15 - ($M$3*G15/SQRT($M$1))</f>
-        <v>2.4544999999999999</v>
+        <v>2.454388423679073</v>
       </c>
       <c r="I15">
         <f>AVERAGE(B15:E15)</f>
@@ -1814,7 +1942,7 @@
       </c>
       <c r="J15">
         <f xml:space="preserve"> I15 + ($M$3*G15/SQRT($M$1))</f>
-        <v>4.0454999999999997</v>
+        <v>4.045611576320927</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1839,7 +1967,7 @@
       </c>
       <c r="H16">
         <f xml:space="preserve"> I16 - ($M$3*G16/SQRT($M$1))</f>
-        <v>2.5814357217193056</v>
+        <v>2.5813068844814602</v>
       </c>
       <c r="I16">
         <f>AVERAGE(B16:E16)</f>
@@ -1847,7 +1975,7 @@
       </c>
       <c r="J16">
         <f xml:space="preserve"> I16 + ($M$3*G16/SQRT($M$1))</f>
-        <v>4.4185642782806944</v>
+        <v>4.4186931155185398</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1872,7 +2000,7 @@
       </c>
       <c r="H17">
         <f xml:space="preserve"> I17 - ($M$3*G17/SQRT($M$1))</f>
-        <v>1.7267334715596661</v>
+        <v>1.726519819171187</v>
       </c>
       <c r="I17">
         <f>AVERAGE(B17:E17)</f>
@@ -1880,7 +2008,7 @@
       </c>
       <c r="J17">
         <f xml:space="preserve"> I17 + ($M$3*G17/SQRT($M$1))</f>
-        <v>4.7732665284403337</v>
+        <v>4.7734801808288125</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1892,16 +2020,16 @@
         <v>0.88108248094035158</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:J20" si="4" xml:space="preserve"> AVERAGE(H2:H7)</f>
-        <v>1.4731977728239007</v>
+        <f xml:space="preserve"> AVERAGE(H2:H7)</f>
+        <v>1.473001156940587</v>
       </c>
       <c r="I20">
-        <f t="shared" si="4"/>
+        <f xml:space="preserve"> AVERAGE(I2:I7)</f>
         <v>2.875</v>
       </c>
       <c r="J20">
-        <f t="shared" si="4"/>
-        <v>4.2768022271760993</v>
+        <f xml:space="preserve"> AVERAGE(J2:J7)</f>
+        <v>4.2769988430594124</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1913,16 +2041,16 @@
         <v>1.3961624188737989</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H21:J21" si="5" xml:space="preserve"> AVERAGE(H8:H13)</f>
-        <v>2.6120389249051192</v>
+        <f xml:space="preserve"> AVERAGE(H8:H13)</f>
+        <v>2.6117273675728896</v>
       </c>
       <c r="I21">
-        <f t="shared" si="5"/>
+        <f xml:space="preserve"> AVERAGE(I8:I13)</f>
         <v>4.833333333333333</v>
       </c>
       <c r="J21">
-        <f t="shared" si="5"/>
-        <v>7.0546277417615473</v>
+        <f xml:space="preserve"> AVERAGE(J8:J13)</f>
+        <v>7.0549392990937774</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1934,16 +2062,16 @@
         <v>0.83052127718757374</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22:J22" si="6" xml:space="preserve"> AVERAGE(H14:H16)</f>
-        <v>1.9286406479945704</v>
+        <f xml:space="preserve"> AVERAGE(H14:H16)</f>
+        <v>1.9284553149774493</v>
       </c>
       <c r="I22">
-        <f t="shared" si="6"/>
+        <f xml:space="preserve"> AVERAGE(I14:I16)</f>
         <v>3.25</v>
       </c>
       <c r="J22">
-        <f t="shared" si="6"/>
-        <v>4.5713593520054294</v>
+        <f xml:space="preserve"> AVERAGE(J14:J16)</f>
+        <v>4.571544685022551</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1955,357 +2083,189 @@
         <v>1.0695287711377477</v>
       </c>
       <c r="H23">
-        <f t="shared" ref="H23:J23" si="7" xml:space="preserve"> AVERAGE(H2:H17)</f>
-        <v>2.0015047251198435</v>
+        <f xml:space="preserve"> AVERAGE(H2:H17)</f>
+        <v>2.0012660569490244</v>
       </c>
       <c r="I23">
-        <f t="shared" si="7"/>
+        <f xml:space="preserve"> AVERAGE(I2:I17)</f>
         <v>3.703125</v>
       </c>
       <c r="J23">
-        <f t="shared" si="7"/>
-        <v>5.4047452748801561</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
-        <v>1</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32">
-        <v>2</v>
-      </c>
-      <c r="G32">
-        <f t="shared" ref="G32:G41" si="8">_xlfn.STDEV.S(B32:E32)</f>
-        <v>0.57735026918962573</v>
-      </c>
-      <c r="H32">
-        <f t="shared" ref="H32:H41" si="9" xml:space="preserve"> I32 - ($M$3*G32/SQRT($M$1))</f>
-        <v>0.58143572171930546</v>
-      </c>
-      <c r="I32">
-        <f t="shared" ref="I32:I41" si="10">AVERAGE(B32:E32)</f>
-        <v>1.5</v>
-      </c>
-      <c r="J32">
-        <f xml:space="preserve"> I32 + ($M$3*G32/SQRT($M$1))</f>
-        <v>2.4185642782806944</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
-        <v>2</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="8"/>
-        <v>0.57735026918962573</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="9"/>
-        <v>0.58143572171930546</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="J33">
-        <f t="shared" ref="J33:J41" si="11" xml:space="preserve"> I33 + ($M$3*G33/SQRT($M$1))</f>
-        <v>2.4185642782806944</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
-        <v>3</v>
-      </c>
-      <c r="B34">
-        <v>3</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
-      </c>
-      <c r="D34">
-        <v>5</v>
-      </c>
-      <c r="E34">
-        <v>6</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="8"/>
-        <v>1.2909944487358056</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="9"/>
-        <v>2.4460278320613331</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="10"/>
-        <v>4.5</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="11"/>
-        <v>6.5539721679386673</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
-        <v>4</v>
-      </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-      <c r="D35">
-        <v>5</v>
-      </c>
-      <c r="E35">
-        <v>6</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="8"/>
-        <v>1.2909944487358056</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="9"/>
-        <v>2.4460278320613331</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="10"/>
-        <v>4.5</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="11"/>
-        <v>6.5539721679386673</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
-        <v>5</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>3</v>
-      </c>
-      <c r="E36">
-        <v>3</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="8"/>
-        <v>0.9574271077563381</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="9"/>
-        <v>0.72673347155966606</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="10"/>
-        <v>2.25</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="11"/>
-        <v>3.7732665284403337</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
-        <v>6</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="D37">
-        <v>3</v>
-      </c>
-      <c r="E37">
-        <v>5</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="8"/>
-        <v>1.6329931618554521</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="9"/>
-        <v>0.40190787948797579</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="11"/>
-        <v>5.5980921205120246</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
-        <v>7</v>
-      </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="D38">
-        <v>3</v>
-      </c>
-      <c r="E38">
-        <v>5</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="8"/>
-        <v>1.2583057392117916</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="9"/>
-        <v>1.2480355689140397</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="10"/>
-        <v>3.25</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="11"/>
-        <v>5.2519644310859608</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
-        <v>8</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-      <c r="D39">
-        <v>3</v>
-      </c>
-      <c r="E39">
-        <v>5</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="8"/>
-        <v>1.2583057392117916</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="9"/>
-        <v>1.2480355689140397</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="10"/>
-        <v>3.25</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="11"/>
-        <v>5.2519644310859608</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
-        <v>9</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40">
-        <v>4</v>
-      </c>
-      <c r="E40">
-        <v>5</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="8"/>
-        <v>1.8257418583505538</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="9"/>
-        <v>9.5244703364269157E-2</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="11"/>
-        <v>5.9047552966357308</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="5">
-        <v>10</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41">
-        <v>2</v>
-      </c>
-      <c r="E41">
-        <v>3</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="8"/>
-        <v>0.81649658092772603</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="9"/>
-        <v>0.7009539397439879</v>
-      </c>
-      <c r="I41">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="11"/>
-        <v>3.2990460602560123</v>
-      </c>
+        <f xml:space="preserve"> AVERAGE(J2:J17)</f>
+        <v>5.4049839430509747</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="8"/>
+      <c r="B85" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2314,4 +2274,1652 @@
     <ignoredError sqref="I3:I4 I5:I14 G3:G14" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <f>_xlfn.STDEV.S(B3:E3)</f>
+        <v>0.57735026918962573</v>
+      </c>
+      <c r="H3">
+        <f xml:space="preserve"> I3 - (PSSUQ!$M$3*G3/SQRT(PSSUQ!$M$1))</f>
+        <v>0.5813068844814604</v>
+      </c>
+      <c r="I3">
+        <f>AVERAGE(B3:E3)</f>
+        <v>1.5</v>
+      </c>
+      <c r="J3">
+        <f xml:space="preserve"> I3 + (PSSUQ!$M$3*G3/SQRT(PSSUQ!$M$1))</f>
+        <v>2.4186931155185398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <f>_xlfn.STDEV.S(B4:E4)</f>
+        <v>0.57735026918962573</v>
+      </c>
+      <c r="H4">
+        <f xml:space="preserve"> I4 - (PSSUQ!$M$3*G4/SQRT(PSSUQ!$M$1))</f>
+        <v>0.5813068844814604</v>
+      </c>
+      <c r="I4">
+        <f>AVERAGE(B4:E4)</f>
+        <v>1.5</v>
+      </c>
+      <c r="J4">
+        <f xml:space="preserve"> I4 + (PSSUQ!$M$3*G4/SQRT(PSSUQ!$M$1))</f>
+        <v>2.4186931155185398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <f>_xlfn.STDEV.S(B5:E5)</f>
+        <v>1.2909944487358056</v>
+      </c>
+      <c r="H5">
+        <f xml:space="preserve"> I5 - (PSSUQ!$M$3*G5/SQRT(PSSUQ!$M$1))</f>
+        <v>2.4457397432394785</v>
+      </c>
+      <c r="I5">
+        <f>AVERAGE(B5:E5)</f>
+        <v>4.5</v>
+      </c>
+      <c r="J5">
+        <f xml:space="preserve"> I5 + (PSSUQ!$M$3*G5/SQRT(PSSUQ!$M$1))</f>
+        <v>6.5542602567605215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <f>_xlfn.STDEV.S(B6:E6)</f>
+        <v>1.2909944487358056</v>
+      </c>
+      <c r="H6">
+        <f xml:space="preserve"> I6 - (PSSUQ!$M$3*G6/SQRT(PSSUQ!$M$1))</f>
+        <v>2.4457397432394785</v>
+      </c>
+      <c r="I6">
+        <f>AVERAGE(B6:E6)</f>
+        <v>4.5</v>
+      </c>
+      <c r="J6">
+        <f xml:space="preserve"> I6 + (PSSUQ!$M$3*G6/SQRT(PSSUQ!$M$1))</f>
+        <v>6.5542602567605215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <f>_xlfn.STDEV.S(B7:E7)</f>
+        <v>0.9574271077563381</v>
+      </c>
+      <c r="H7">
+        <f xml:space="preserve"> I7 - (PSSUQ!$M$3*G7/SQRT(PSSUQ!$M$1))</f>
+        <v>0.72651981917118702</v>
+      </c>
+      <c r="I7">
+        <f>AVERAGE(B7:E7)</f>
+        <v>2.25</v>
+      </c>
+      <c r="J7">
+        <f xml:space="preserve"> I7 + (PSSUQ!$M$3*G7/SQRT(PSSUQ!$M$1))</f>
+        <v>3.773480180828813</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <f>_xlfn.STDEV.S(B8:E8)</f>
+        <v>1.6329931618554521</v>
+      </c>
+      <c r="H8">
+        <f xml:space="preserve"> I8 - (PSSUQ!$M$3*G8/SQRT(PSSUQ!$M$1))</f>
+        <v>0.40154347274977731</v>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(B8:E8)</f>
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <f xml:space="preserve"> I8 + (PSSUQ!$M$3*G8/SQRT(PSSUQ!$M$1))</f>
+        <v>5.5984565272502227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <f>_xlfn.STDEV.S(B9:E9)</f>
+        <v>1.2583057392117916</v>
+      </c>
+      <c r="H9">
+        <f xml:space="preserve"> I9 - (PSSUQ!$M$3*G9/SQRT(PSSUQ!$M$1))</f>
+        <v>1.2477547746640738</v>
+      </c>
+      <c r="I9">
+        <f>AVERAGE(B9:E9)</f>
+        <v>3.25</v>
+      </c>
+      <c r="J9">
+        <f xml:space="preserve"> I9 + (PSSUQ!$M$3*G9/SQRT(PSSUQ!$M$1))</f>
+        <v>5.2522452253359262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <f>_xlfn.STDEV.S(B10:E10)</f>
+        <v>1.2583057392117916</v>
+      </c>
+      <c r="H10">
+        <f xml:space="preserve"> I10 - (PSSUQ!$M$3*G10/SQRT(PSSUQ!$M$1))</f>
+        <v>1.2477547746640738</v>
+      </c>
+      <c r="I10">
+        <f>AVERAGE(B10:E10)</f>
+        <v>3.25</v>
+      </c>
+      <c r="J10">
+        <f xml:space="preserve"> I10 + (PSSUQ!$M$3*G10/SQRT(PSSUQ!$M$1))</f>
+        <v>5.2522452253359262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <f>_xlfn.STDEV.S(B11:E11)</f>
+        <v>1.8257418583505538</v>
+      </c>
+      <c r="H11">
+        <f xml:space="preserve"> I11 - (PSSUQ!$M$3*G11/SQRT(PSSUQ!$M$1))</f>
+        <v>9.4837284245233633E-2</v>
+      </c>
+      <c r="I11">
+        <f>AVERAGE(B11:E11)</f>
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <f xml:space="preserve"> I11 + (PSSUQ!$M$3*G11/SQRT(PSSUQ!$M$1))</f>
+        <v>5.9051627157547664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <f>_xlfn.STDEV.S(B12:E12)</f>
+        <v>0.81649658092772603</v>
+      </c>
+      <c r="H12">
+        <f xml:space="preserve"> I12 - (PSSUQ!$M$3*G12/SQRT(PSSUQ!$M$1))</f>
+        <v>0.70077173637488865</v>
+      </c>
+      <c r="I12">
+        <f>AVERAGE(B12:E12)</f>
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <f xml:space="preserve"> I12 + (PSSUQ!$M$3*G12/SQRT(PSSUQ!$M$1))</f>
+        <v>3.2992282636251113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>2</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>2</v>
+      </c>
+      <c r="T2">
+        <v>2</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>2</v>
+      </c>
+      <c r="W2">
+        <v>2</v>
+      </c>
+      <c r="X2">
+        <v>2</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>2</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>2</v>
+      </c>
+      <c r="AC3">
+        <v>2</v>
+      </c>
+      <c r="AD3">
+        <v>2</v>
+      </c>
+      <c r="AE3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>4</v>
+      </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
+      <c r="T4">
+        <v>3</v>
+      </c>
+      <c r="U4">
+        <v>4</v>
+      </c>
+      <c r="V4">
+        <v>3</v>
+      </c>
+      <c r="W4">
+        <v>3</v>
+      </c>
+      <c r="X4">
+        <v>4</v>
+      </c>
+      <c r="Y4">
+        <v>3</v>
+      </c>
+      <c r="Z4">
+        <v>3</v>
+      </c>
+      <c r="AA4">
+        <v>3</v>
+      </c>
+      <c r="AB4">
+        <v>3</v>
+      </c>
+      <c r="AC4">
+        <v>2</v>
+      </c>
+      <c r="AD4">
+        <v>4</v>
+      </c>
+      <c r="AE4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>4</v>
+      </c>
+      <c r="Y5">
+        <v>3</v>
+      </c>
+      <c r="Z5">
+        <v>4</v>
+      </c>
+      <c r="AA5">
+        <v>5</v>
+      </c>
+      <c r="AB5">
+        <v>3</v>
+      </c>
+      <c r="AC5">
+        <v>3</v>
+      </c>
+      <c r="AD5">
+        <v>4</v>
+      </c>
+      <c r="AE5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15">
+        <f>AVERAGE(B2:B6)</f>
+        <v>2.75</v>
+      </c>
+      <c r="C15">
+        <f>AVERAGE(C2:C6)</f>
+        <v>2.75</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(D2:D6)</f>
+        <v>2.5</v>
+      </c>
+      <c r="E15">
+        <f>AVERAGE(E2:E6)</f>
+        <v>2.25</v>
+      </c>
+      <c r="F15">
+        <f>AVERAGE(F2:F6)</f>
+        <v>2.75</v>
+      </c>
+      <c r="G15">
+        <f>AVERAGE(G2:G6)</f>
+        <v>2.25</v>
+      </c>
+      <c r="H15">
+        <f>AVERAGE(H2:H6)</f>
+        <v>3.25</v>
+      </c>
+      <c r="I15">
+        <f>AVERAGE(I2:I6)</f>
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <f>AVERAGE(J2:J6)</f>
+        <v>3.5</v>
+      </c>
+      <c r="K15">
+        <f>AVERAGE(K2:K5)</f>
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <f>AVERAGE(L2:L6)</f>
+        <v>4.5</v>
+      </c>
+      <c r="M15">
+        <f>AVERAGE(M2:M6)</f>
+        <v>2.75</v>
+      </c>
+      <c r="N15">
+        <f>AVERAGE(N2:N6)</f>
+        <v>2.5</v>
+      </c>
+      <c r="O15">
+        <f>AVERAGE(O2:O6)</f>
+        <v>2.75</v>
+      </c>
+      <c r="P15">
+        <f>AVERAGE(P2:P6)</f>
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <f>AVERAGE(Q2:Q6)</f>
+        <v>2.25</v>
+      </c>
+      <c r="R15">
+        <f>AVERAGE(R2:R5)</f>
+        <v>3.25</v>
+      </c>
+      <c r="S15">
+        <f>AVERAGE(S2:S5)</f>
+        <v>2.75</v>
+      </c>
+      <c r="T15">
+        <f>AVERAGE(T2:T5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="U15">
+        <f>AVERAGE(U2:U5)</f>
+        <v>3</v>
+      </c>
+      <c r="V15">
+        <f>AVERAGE(V2:V5)</f>
+        <v>2.75</v>
+      </c>
+      <c r="W15">
+        <f>AVERAGE(W2:W5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="X15">
+        <f>AVERAGE(X2:X5)</f>
+        <v>3</v>
+      </c>
+      <c r="Y15">
+        <f>AVERAGE(Y2:Y5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="Z15">
+        <f>AVERAGE(Z2:Z5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="AA15">
+        <f>AVERAGE(AA2:AA5)</f>
+        <v>2.5</v>
+      </c>
+      <c r="AB15">
+        <f>AVERAGE(AB2:AB5)</f>
+        <v>2.25</v>
+      </c>
+      <c r="AC15">
+        <f>AVERAGE(AC2:AC5)</f>
+        <v>2</v>
+      </c>
+      <c r="AD15">
+        <f>AVERAGE(AD2:AD5)</f>
+        <v>3</v>
+      </c>
+      <c r="AE15">
+        <f>AVERAGE(AE2:AE5)</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16">
+        <f>AVERAGE(B15:D15)</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="F16">
+        <f>AVERAGE(E15:G15)</f>
+        <v>2.4166666666666665</v>
+      </c>
+      <c r="I16">
+        <f>AVERAGE(H15:J15)</f>
+        <v>3.5833333333333335</v>
+      </c>
+      <c r="L16">
+        <f>AVERAGE(K15:M15)</f>
+        <v>3.75</v>
+      </c>
+      <c r="O16">
+        <f>AVERAGE(N15:P15)</f>
+        <v>2.75</v>
+      </c>
+      <c r="R16">
+        <f>AVERAGE(Q15:S15)</f>
+        <v>2.75</v>
+      </c>
+      <c r="U16">
+        <f>AVERAGE(T15:V15)</f>
+        <v>2.75</v>
+      </c>
+      <c r="X16">
+        <f>AVERAGE(W15:Y15)</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="AA16">
+        <f>AVERAGE(Z15:AB15)</f>
+        <v>2.4166666666666665</v>
+      </c>
+      <c r="AD16">
+        <f>AVERAGE(AC15:AE15)</f>
+        <v>2.5833333333333335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18">
+        <f>_xlfn.STDEV.S(B2:D5)</f>
+        <v>1.1547005383792517</v>
+      </c>
+      <c r="F18">
+        <f>_xlfn.STDEV.S(E2:G5)</f>
+        <v>1.083624669450832</v>
+      </c>
+      <c r="I18">
+        <f>_xlfn.STDEV.S(H2:J5)</f>
+        <v>1.0836246694508314</v>
+      </c>
+      <c r="L18">
+        <f>_xlfn.STDEV.S(K2:M5)</f>
+        <v>1.1381803659589922</v>
+      </c>
+      <c r="O18">
+        <f>_xlfn.STDEV.S(N2:P5)</f>
+        <v>1.0552897060221726</v>
+      </c>
+      <c r="R18">
+        <f>_xlfn.STDEV.S(Q2:S5)</f>
+        <v>1.1381803659589922</v>
+      </c>
+      <c r="U18">
+        <f>_xlfn.STDEV.S(T2:V5)</f>
+        <v>0.75377836144440913</v>
+      </c>
+      <c r="X18">
+        <f>_xlfn.STDEV.S(W2:Y5)</f>
+        <v>0.88762536459859476</v>
+      </c>
+      <c r="AA18">
+        <f>_xlfn.STDEV.S(Z2:AB5)</f>
+        <v>1.3113721705515067</v>
+      </c>
+      <c r="AD18">
+        <f>_xlfn.STDEV.S(AC2:AE5)</f>
+        <v>1.2401124093721456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19">
+        <f>_xlfn.SKEW.P(B2:D5)</f>
+        <v>-5.4820244468683776E-2</v>
+      </c>
+      <c r="F19">
+        <f>_xlfn.SKEW.P(E2:G5)</f>
+        <v>-1.0364120372929493E-3</v>
+      </c>
+      <c r="I19">
+        <f>_xlfn.SKEW.P(H2:J5)</f>
+        <v>1.0364120372931367E-3</v>
+      </c>
+      <c r="L19">
+        <f>_xlfn.SKEW.P(K2:M5)</f>
+        <v>-1.0384080585720157</v>
+      </c>
+      <c r="O19">
+        <f>_xlfn.SKEW.P(N2:P5)</f>
+        <v>0.99984274022926467</v>
+      </c>
+      <c r="R19">
+        <f>_xlfn.SKEW.P(Q2:S5)</f>
+        <v>0.12074512308976931</v>
+      </c>
+      <c r="U19">
+        <f>_xlfn.SKEW.P(T2:V5)</f>
+        <v>0.41569219381653061</v>
+      </c>
+      <c r="X19">
+        <f>_xlfn.SKEW.P(W2:Y5)</f>
+        <v>-0.12068685239272803</v>
+      </c>
+      <c r="AA19">
+        <f>_xlfn.SKEW.P(Z2:AB5)</f>
+        <v>0.44150757731980517</v>
+      </c>
+      <c r="AD19">
+        <f>_xlfn.SKEW.P(AC2:AE5)</f>
+        <v>0.54835161402016885</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20">
+        <f>KURT(B2:D5)</f>
+        <v>-1.4727272727272736</v>
+      </c>
+      <c r="F20">
+        <f>KURT(E2:G5)</f>
+        <v>-1.1526992715920934</v>
+      </c>
+      <c r="I20">
+        <f>KURT(H2:J5)</f>
+        <v>-1.1526992715920912</v>
+      </c>
+      <c r="L20">
+        <f>KURT(K2:M5)</f>
+        <v>2.1153585718682679</v>
+      </c>
+      <c r="O20">
+        <f>KURT(N2:P5)</f>
+        <v>0.12583645703179247</v>
+      </c>
+      <c r="R20">
+        <f>KURT(Q2:S5)</f>
+        <v>0.42523853493382546</v>
+      </c>
+      <c r="U20">
+        <f>KURT(T2:V5)</f>
+        <v>-0.86826666666666874</v>
+      </c>
+      <c r="X20">
+        <f>KURT(W2:Y5)</f>
+        <v>-0.25384615384615472</v>
+      </c>
+      <c r="AA20">
+        <f>KURT(Z2:AB5)</f>
+        <v>-0.43906926196898954</v>
+      </c>
+      <c r="AD20">
+        <f>KURT(AC2:AE5)</f>
+        <v>-0.34402193695551775</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9">
+        <v>2</v>
+      </c>
+      <c r="D23" s="9">
+        <v>3</v>
+      </c>
+      <c r="E23" s="9">
+        <v>4</v>
+      </c>
+      <c r="F23" s="9">
+        <v>5</v>
+      </c>
+      <c r="G23" s="9">
+        <v>6</v>
+      </c>
+      <c r="H23" s="9">
+        <v>7</v>
+      </c>
+      <c r="I23" s="9">
+        <v>8</v>
+      </c>
+      <c r="J23" s="9">
+        <v>9</v>
+      </c>
+      <c r="K23" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f>CORREL(B$15:D$15,$B$15:$D$15)</f>
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f>CORREL(E$15:G$15,$B$15:$D$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D24">
+        <f>CORREL($H$15:$J$15,$B$15:$D$15)</f>
+        <v>0.18898223650461363</v>
+      </c>
+      <c r="E24">
+        <f>CORREL($K15:$M15,$B$15:$D$15)</f>
+        <v>0.96076892283052284</v>
+      </c>
+      <c r="F24">
+        <f>CORREL($N15:$P15,$B$15:$D$15)</f>
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="G24">
+        <f>CORREL($Q$15:$S$15,$B$15:$D$15)</f>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f>CORREL($T$15:$V$15,$B$15:$D$15)</f>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f>CORREL($W$15:$Y$15,$B$15:$D$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J24">
+        <f>CORREL($Z$15:$AB$15,$B$15:$D$15)</f>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f>CORREL($AC$15:$AE$15,$B$15:$D$15)</f>
+        <v>-0.27735009811261452</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>0.5</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f>CORREL($H$15:$J$15,$E$15:$G$15)</f>
+        <v>0.94491118252306794</v>
+      </c>
+      <c r="E25">
+        <f>CORREL($K15:$M15,$E$15:$G$15)</f>
+        <v>0.72057669212289222</v>
+      </c>
+      <c r="F25">
+        <f>CORREL($N15:$P15,$E$15:$G$15)</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>CORREL($Q$15:$S$15,$E$15:$G$15)</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="H25">
+        <f>CORREL($T$15:$V$15,$E$15:$G$15)</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="I25">
+        <f>CORREL($W$15:$Y$15,$E$15:$G$15)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="J25">
+        <f>CORREL($Z$15:$AB$15,$E$15:$G$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K25">
+        <f>CORREL($AC$15:$AE$15,$E$15:$G$15)</f>
+        <v>0.69337524528153627</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <f>CORREL($H$15:$J$15,$B$15:$D$15)</f>
+        <v>0.18898223650461363</v>
+      </c>
+      <c r="C26">
+        <f>CORREL($H$15:$J$15,$E$15:$G$15)</f>
+        <v>0.94491118252306794</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f>CORREL($K15:$M15,$H$15:$J$15)</f>
+        <v>0.45392064950160188</v>
+      </c>
+      <c r="F26">
+        <f>CORREL($N15:$P15,$H$15:$J$15)</f>
+        <v>0.3273268353539886</v>
+      </c>
+      <c r="G26">
+        <f>CORREL($Q$15:$S$15,$H$15:$J$15)</f>
+        <v>0.98198050606196585</v>
+      </c>
+      <c r="H26">
+        <f>CORREL($T$15:$V$15,$H$15:$J$15)</f>
+        <v>0.98198050606196585</v>
+      </c>
+      <c r="I26">
+        <f>CORREL($W$15:$Y$15,$H$15:$J$15)</f>
+        <v>0.94491118252306794</v>
+      </c>
+      <c r="J26">
+        <f>CORREL($Z$15:$AB$15,$H$15:$J$15)</f>
+        <v>0.18898223650461363</v>
+      </c>
+      <c r="K26">
+        <f>CORREL($AC$15:$AE$15,$H$15:$J$15)</f>
+        <v>0.89104211121363075</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <f>CORREL($K15:$M15,$B$15:$D$15)</f>
+        <v>0.96076892283052284</v>
+      </c>
+      <c r="C27">
+        <f>CORREL($K15:$M15,$E$15:$G$15)</f>
+        <v>0.72057669212289222</v>
+      </c>
+      <c r="D27">
+        <f>CORREL($K15:$M15,$H$15:$J$15)</f>
+        <v>0.45392064950160188</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f>CORREL($N15:$P15,$K$15:$M$15)</f>
+        <v>-0.69337524528153638</v>
+      </c>
+      <c r="G27">
+        <f>CORREL($Q$15:$S$15,$K$15:$M$15)</f>
+        <v>0.27735009811261452</v>
+      </c>
+      <c r="H27">
+        <f>CORREL($T$15:$V$15,$K$15:$M$15)</f>
+        <v>0.27735009811261452</v>
+      </c>
+      <c r="I27">
+        <f>CORREL($W$15:$Y$15,$K$15:$M$15)</f>
+        <v>0.72057669212289222</v>
+      </c>
+      <c r="J27">
+        <f>CORREL($Z$15:$AB$15,$K$15:$M$15)</f>
+        <v>0.96076892283052284</v>
+      </c>
+      <c r="K27">
+        <f>CORREL($AC$15:$AE$15,$K$15:$M$15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <f>CORREL($N15:$P15,$B$15:$D$15)</f>
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="C28">
+        <f>CORREL($N15:$P15,$E$15:$G$15)</f>
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f>CORREL($N15:$P15,$H$15:$J$15)</f>
+        <v>0.3273268353539886</v>
+      </c>
+      <c r="E28">
+        <f>CORREL($N15:$P15,$K$15:$M$15)</f>
+        <v>-0.69337524528153638</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f>CORREL($Q$15:$S$15,$N$15:$P$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H28">
+        <f>CORREL($T$15:$V$15,$N$15:$P$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I28">
+        <f>CORREL($W$15:$Y$15,$N$15:$P$15)</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f>CORREL($Z$15:$AB$15,$N$15:$P$15)</f>
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="K28">
+        <f>CORREL($AC$15:$AE$15,$N$15:$P$15)</f>
+        <v>0.7205766921228921</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <f>CORREL($Q$15:$S$15,$B$15:$D$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f>CORREL($Q$15:$S$15,$E$15:$G$15)</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="D29">
+        <f>CORREL($Q$15:$S$15,$H$15:$J$15)</f>
+        <v>0.98198050606196585</v>
+      </c>
+      <c r="E29">
+        <f>CORREL($Q$15:$S$15,$K$15:$M$15)</f>
+        <v>0.27735009811261452</v>
+      </c>
+      <c r="F29">
+        <f>CORREL($Q$15:$S$15,$N$15:$P$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f>CORREL($T$15:$V$15,$Q$15:$S$15)</f>
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <f>CORREL($W$15:$Y$15,$Q$15:$S$15)</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="J29">
+        <f>CORREL($Z$15:$AB$15,$Q$15:$S$15)</f>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f>CORREL($AC$15:$AE$15,$Q$15:$S$15)</f>
+        <v>0.96076892283052273</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <f>CORREL($T$15:$V$15,$B$15:$D$15)</f>
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f>CORREL($T$15:$V$15,$E$15:$G$15)</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="D30">
+        <f>CORREL($T$15:$V$15,$H$15:$J$15)</f>
+        <v>0.98198050606196585</v>
+      </c>
+      <c r="E30">
+        <f>CORREL($T$15:$V$15,$K$15:$M$15)</f>
+        <v>0.27735009811261452</v>
+      </c>
+      <c r="F30">
+        <f>CORREL($T$15:$V$15,$N$15:$P$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G30">
+        <f>CORREL($T$15:$V$15,$Q$15:$S$15)</f>
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <f>CORREL($W$15:$Y$15,$T$15:$V$15)</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="J30">
+        <f>CORREL($Z$15:$AB$15,$Q$15:$S$15)</f>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f>CORREL($AC$15:$AE$15,$Q$15:$S$15)</f>
+        <v>0.96076892283052273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <f>CORREL($W$15:$Y$15,$B$15:$D$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C31">
+        <f>CORREL($W$15:$Y$15,$E$15:$G$15)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D31">
+        <f>CORREL($W$15:$Y$15,$H$15:$J$15)</f>
+        <v>0.94491118252306794</v>
+      </c>
+      <c r="E31">
+        <f>CORREL($W$15:$Y$15,$K$15:$M$15)</f>
+        <v>0.72057669212289222</v>
+      </c>
+      <c r="F31">
+        <f>CORREL($W$15:$Y$15,$N$15:$P$15)</f>
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <f>CORREL($W$15:$Y$15,$Q$15:$S$15)</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="H31">
+        <f>CORREL($W$15:$Y$15,$T$15:$V$15)</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <f>CORREL($Z$15:$AB$15,$W$15:$Y$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K31">
+        <f>CORREL($AC$15:$AE$15,$W$15:$Y$15)</f>
+        <v>0.69337524528153627</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <f>CORREL($Z$15:$AB$15,$B$15:$D$15)</f>
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <f>CORREL($Z$15:$AB$15,$E$15:$G$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D32">
+        <f>CORREL($Z$15:$AB$15,$H$15:$J$15)</f>
+        <v>0.18898223650461363</v>
+      </c>
+      <c r="E32">
+        <f>CORREL($Z$15:$AB$15,$K$15:$M$15)</f>
+        <v>0.96076892283052284</v>
+      </c>
+      <c r="F32">
+        <f>CORREL($Z$15:$AB$15,$N$15:$P$15)</f>
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="G32">
+        <f>CORREL($Z$15:$AB$15,$Q$15:$S$15)</f>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f>CORREL($Z$15:$AB$15,$Q$15:$S$15)</f>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f>CORREL($Z$15:$AB$15,$W$15:$Y$15)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <f>CORREL($AC$15:$AE$15,$Z$15:$AB$15)</f>
+        <v>-0.27735009811261452</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <f>CORREL($AC$15:$AE$15,$B$15:$D$15)</f>
+        <v>-0.27735009811261452</v>
+      </c>
+      <c r="C33">
+        <f>CORREL($AC$15:$AE$15,$E$15:$G$15)</f>
+        <v>0.69337524528153627</v>
+      </c>
+      <c r="D33">
+        <f>CORREL($AC$15:$AE$15,$H$15:$J$15)</f>
+        <v>0.89104211121363075</v>
+      </c>
+      <c r="E33">
+        <f>CORREL($AC$15:$AE$15,$K$15:$M$15)</f>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f>CORREL($AC$15:$AE$15,$N$15:$P$15)</f>
+        <v>0.7205766921228921</v>
+      </c>
+      <c r="G33">
+        <f>CORREL($AC$15:$AE$15,$Q$15:$S$15)</f>
+        <v>0.96076892283052273</v>
+      </c>
+      <c r="H33">
+        <f>CORREL($AC$15:$AE$15,$Q$15:$S$15)</f>
+        <v>0.96076892283052273</v>
+      </c>
+      <c r="I33">
+        <f>CORREL($AC$15:$AE$15,$W$15:$Y$15)</f>
+        <v>0.69337524528153627</v>
+      </c>
+      <c r="J33">
+        <f>CORREL($AC$15:$AE$15,$Z$15:$AB$15)</f>
+        <v>-0.27735009811261452</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
alle data in excel
</commit_message>
<xml_diff>
--- a/pract3/Gebruiksreview Body Photo Browser (Reacties).xlsx
+++ b/pract3/Gebruiksreview Body Photo Browser (Reacties).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Formulierreacties 1" sheetId="1" r:id="rId1"/>
@@ -1437,79 +1437,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J41" sqref="A30:J41"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="M1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(B3)</f>
         <v>2</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
       <c r="G2">
-        <f>_xlfn.STDEV.S(B2:E2)</f>
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <f xml:space="preserve"> I2 - ($M$3*G2/SQRT($M$1))</f>
-        <v>1.9543884236790727</v>
-      </c>
-      <c r="I2">
-        <f>AVERAGE(B2:E2)</f>
-        <v>2.75</v>
-      </c>
-      <c r="J2">
-        <f xml:space="preserve"> I2 + ($M$3*G2/SQRT($M$1))</f>
-        <v>3.545611576320927</v>
-      </c>
-      <c r="L2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <f>_xlfn.STDEV.S(B2:H2)</f>
+        <v>0.5345224838248489</v>
+      </c>
+      <c r="M2">
+        <f xml:space="preserve"> N2 - ($R$3*L2/SQRT($R$1))</f>
+        <v>2.077077724882761</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(B2:H2)</f>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="O2">
+        <f xml:space="preserve"> N2 + ($R$3*L2/SQRT($R$1))</f>
+        <v>3.0657794179743822</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="M2">
-        <f>M1-1</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R2">
+        <f>R1-1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1520,36 +1528,45 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
       </c>
       <c r="G3">
-        <f>_xlfn.STDEV.S(B3:E3)</f>
-        <v>0.9574271077563381</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <f xml:space="preserve"> I3 - ($M$3*G3/SQRT($M$1))</f>
-        <v>1.226519819171187</v>
-      </c>
-      <c r="I3">
-        <f>AVERAGE(B3:E3)</f>
-        <v>2.75</v>
-      </c>
-      <c r="J3">
-        <f xml:space="preserve"> I3 + ($M$3*G3/SQRT($M$1))</f>
-        <v>4.2734801808288125</v>
-      </c>
-      <c r="L3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L17" si="0">_xlfn.STDEV.S(B3:H3)</f>
+        <v>0.7867957924694432</v>
+      </c>
+      <c r="M3">
+        <f xml:space="preserve"> N3 - ($R$3*L3/SQRT($R$1))</f>
+        <v>1.7009066851115402</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N17" si="1">AVERAGE(B3:H3)</f>
+        <v>2.4285714285714284</v>
+      </c>
+      <c r="O3">
+        <f xml:space="preserve"> N3 + ($R$3*L3/SQRT($R$1))</f>
+        <v>3.1562361720313166</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M3">
-        <f>_xlfn.T.INV.2T(0.05, M2)</f>
-        <v>3.1824463052837091</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="R3">
+        <f>_xlfn.T.INV.2T(0.05, R2)</f>
+        <v>2.4469118511449697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1557,7 +1574,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1565,24 +1582,33 @@
       <c r="E4">
         <v>3</v>
       </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
       <c r="G4">
-        <f>_xlfn.STDEV.S(B4:E4)</f>
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <f xml:space="preserve"> I4 - ($M$3*G4/SQRT($M$1))</f>
-        <v>1.9543884236790727</v>
-      </c>
-      <c r="I4">
-        <f>AVERAGE(B4:E4)</f>
-        <v>2.75</v>
-      </c>
-      <c r="J4">
-        <f xml:space="preserve"> I4 + ($M$3*G4/SQRT($M$1))</f>
-        <v>3.545611576320927</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0.48795003647426693</v>
+      </c>
+      <c r="M4">
+        <f xml:space="preserve"> N4 - ($R$3*L4/SQRT($R$1))</f>
+        <v>2.2630071976608557</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="O4">
+        <f xml:space="preserve"> N4 + ($R$3*L4/SQRT($R$1))</f>
+        <v>3.1655642309105732</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1590,65 +1616,83 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
       </c>
       <c r="G5">
-        <f>_xlfn.STDEV.S(B5:E5)</f>
-        <v>1.4142135623730951</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <f xml:space="preserve"> I5 - ($M$3*G5/SQRT($M$1))</f>
-        <v>0.74967063677181534</v>
-      </c>
-      <c r="I5">
-        <f>AVERAGE(B5:E5)</f>
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <f xml:space="preserve"> I5 + ($M$3*G5/SQRT($M$1))</f>
-        <v>5.2503293632281842</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1.0690449676496974</v>
+      </c>
+      <c r="M5">
+        <f xml:space="preserve"> N5 - ($R$3*L5/SQRT($R$1))</f>
+        <v>1.8684411640512368</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="O5">
+        <f xml:space="preserve"> N5 + ($R$3*L5/SQRT($R$1))</f>
+        <v>3.8458445502344776</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="3">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <f>_xlfn.STDEV.S(B6:E6)</f>
-        <v>0.9574271077563381</v>
-      </c>
-      <c r="H6">
-        <f xml:space="preserve"> I6 - ($M$3*G6/SQRT($M$1))</f>
-        <v>1.226519819171187</v>
-      </c>
-      <c r="I6">
-        <f>AVERAGE(B6:E6)</f>
-        <v>2.75</v>
-      </c>
-      <c r="J6">
-        <f xml:space="preserve"> I6 + ($M$3*G6/SQRT($M$1))</f>
-        <v>4.2734801808288125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="12">
+        <v>2</v>
+      </c>
+      <c r="G6" s="12">
+        <v>3</v>
+      </c>
+      <c r="H6" s="12">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>1.1547005383792515</v>
+      </c>
+      <c r="M6">
+        <f xml:space="preserve"> N6 - ($R$3*L6/SQRT($R$1))</f>
+        <v>0.93208011649939615</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <f xml:space="preserve"> N6 + ($R$3*L6/SQRT($R$1))</f>
+        <v>3.0679198835006041</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1664,24 +1708,33 @@
       <c r="E7" s="3">
         <v>4</v>
       </c>
-      <c r="G7">
-        <f>_xlfn.STDEV.S(B7:E7)</f>
-        <v>0.9574271077563381</v>
-      </c>
-      <c r="H7">
-        <f xml:space="preserve"> I7 - ($M$3*G7/SQRT($M$1))</f>
-        <v>1.726519819171187</v>
-      </c>
-      <c r="I7">
-        <f>AVERAGE(B7:E7)</f>
-        <v>3.25</v>
-      </c>
-      <c r="J7">
-        <f xml:space="preserve"> I7 + ($M$3*G7/SQRT($M$1))</f>
-        <v>4.7734801808288125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F7" s="12">
+        <v>4</v>
+      </c>
+      <c r="G7" s="12">
+        <v>4</v>
+      </c>
+      <c r="H7" s="12">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.78679579246944253</v>
+      </c>
+      <c r="M7">
+        <f xml:space="preserve"> N7 - ($R$3*L7/SQRT($R$1))</f>
+        <v>2.8437638279686839</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="O7">
+        <f xml:space="preserve"> N7 + ($R$3*L7/SQRT($R$1))</f>
+        <v>4.2990933148884594</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1692,194 +1745,248 @@
         <v>5</v>
       </c>
       <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6</v>
+      </c>
+      <c r="F8" s="12">
         <v>7</v>
       </c>
-      <c r="E8">
+      <c r="G8" s="12">
         <v>7</v>
       </c>
-      <c r="G8">
-        <f>_xlfn.STDEV.S(B8:E8)</f>
-        <v>1.5</v>
-      </c>
-      <c r="H8">
-        <f xml:space="preserve"> I8 - ($M$3*G8/SQRT($M$1))</f>
-        <v>3.363165271037218</v>
-      </c>
-      <c r="I8">
-        <f>AVERAGE(B8:E8)</f>
-        <v>5.75</v>
-      </c>
-      <c r="J8">
-        <f xml:space="preserve"> I8 + ($M$3*G8/SQRT($M$1))</f>
-        <v>8.136834728962782</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H8" s="12">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>1.2149857925879122</v>
+      </c>
+      <c r="M8">
+        <f xml:space="preserve"> N8 - ($R$3*L8/SQRT($R$1))</f>
+        <v>4.7334684126011011</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>5.8571428571428568</v>
+      </c>
+      <c r="O8">
+        <f xml:space="preserve"> N8 + ($R$3*L8/SQRT($R$1))</f>
+        <v>6.9808173016846125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="12">
+        <v>4</v>
+      </c>
+      <c r="G9" s="12">
+        <v>4</v>
+      </c>
+      <c r="H9" s="12">
         <v>5</v>
       </c>
-      <c r="G9">
-        <f>_xlfn.STDEV.S(B9:E9)</f>
-        <v>0.81649658092772603</v>
-      </c>
-      <c r="H9">
-        <f xml:space="preserve"> I9 - ($M$3*G9/SQRT($M$1))</f>
-        <v>2.7007717363748887</v>
-      </c>
-      <c r="I9">
-        <f>AVERAGE(B9:E9)</f>
-        <v>4</v>
-      </c>
-      <c r="J9">
-        <f xml:space="preserve"> I9 + ($M$3*G9/SQRT($M$1))</f>
-        <v>5.2992282636251113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>1.3451854182690988</v>
+      </c>
+      <c r="M9">
+        <f xml:space="preserve"> N9 - ($R$3*L9/SQRT($R$1))</f>
+        <v>1.8987681280715412</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>3.1428571428571428</v>
+      </c>
+      <c r="O9">
+        <f xml:space="preserve"> N9 + ($R$3*L9/SQRT($R$1))</f>
+        <v>4.3869461576427442</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="12">
+        <v>4</v>
+      </c>
+      <c r="G10" s="12">
         <v>7</v>
       </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <f>_xlfn.STDEV.S(B10:E10)</f>
-        <v>1.7320508075688772</v>
-      </c>
-      <c r="H10">
-        <f xml:space="preserve"> I10 - ($M$3*G10/SQRT($M$1))</f>
-        <v>1.743920653444381</v>
-      </c>
-      <c r="I10">
-        <f>AVERAGE(B10:E10)</f>
-        <v>4.5</v>
-      </c>
-      <c r="J10">
-        <f xml:space="preserve"> I10 + ($M$3*G10/SQRT($M$1))</f>
-        <v>7.2560793465556195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H10" s="12">
+        <v>7</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2.1380899352993947</v>
+      </c>
+      <c r="M10">
+        <f xml:space="preserve"> N10 - ($R$3*L10/SQRT($R$1))</f>
+        <v>2.3083108995310448</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>4.2857142857142856</v>
+      </c>
+      <c r="O10">
+        <f xml:space="preserve"> N10 + ($R$3*L10/SQRT($R$1))</f>
+        <v>6.2631176718975263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" s="12">
         <v>5</v>
       </c>
-      <c r="E11">
+      <c r="G11" s="12">
         <v>7</v>
       </c>
-      <c r="G11">
-        <f>_xlfn.STDEV.S(B11:E11)</f>
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="H11">
-        <f xml:space="preserve"> I11 - ($M$3*G11/SQRT($M$1))</f>
-        <v>2.7496706367718153</v>
-      </c>
-      <c r="I11">
-        <f>AVERAGE(B11:E11)</f>
-        <v>5</v>
-      </c>
-      <c r="J11">
-        <f xml:space="preserve"> I11 + ($M$3*G11/SQRT($M$1))</f>
-        <v>7.2503293632281842</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H11" s="12">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>1.8257418583505538</v>
+      </c>
+      <c r="M11">
+        <f xml:space="preserve"> N11 - ($R$3*L11/SQRT($R$1))</f>
+        <v>2.3114704047782109</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <f xml:space="preserve"> N11 + ($R$3*L11/SQRT($R$1))</f>
+        <v>5.6885295952217891</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" s="12">
+        <v>4</v>
+      </c>
+      <c r="G12" s="12">
+        <v>4</v>
+      </c>
+      <c r="H12" s="12">
         <v>7</v>
       </c>
-      <c r="G12">
-        <f>_xlfn.STDEV.S(B12:E12)</f>
-        <v>1.5</v>
-      </c>
-      <c r="H12">
-        <f xml:space="preserve"> I12 - ($M$3*G12/SQRT($M$1))</f>
-        <v>2.363165271037218</v>
-      </c>
-      <c r="I12">
-        <f>AVERAGE(B12:E12)</f>
-        <v>4.75</v>
-      </c>
-      <c r="J12">
-        <f xml:space="preserve"> I12 + ($M$3*G12/SQRT($M$1))</f>
-        <v>7.136834728962782</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>1.9880595947760096</v>
+      </c>
+      <c r="M12">
+        <f xml:space="preserve"> N12 - ($R$3*L12/SQRT($R$1))</f>
+        <v>1.5899229649399482</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="O12">
+        <f xml:space="preserve"> N12 + ($R$3*L12/SQRT($R$1))</f>
+        <v>5.2672198922029088</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" s="12">
         <v>5</v>
       </c>
-      <c r="D13">
+      <c r="G13" s="12">
         <v>7</v>
       </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-      <c r="G13">
-        <f>_xlfn.STDEV.S(B13:E13)</f>
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="H13">
-        <f xml:space="preserve"> I13 - ($M$3*G13/SQRT($M$1))</f>
-        <v>2.7496706367718153</v>
-      </c>
-      <c r="I13">
-        <f>AVERAGE(B13:E13)</f>
-        <v>5</v>
-      </c>
-      <c r="J13">
-        <f xml:space="preserve"> I13 + ($M$3*G13/SQRT($M$1))</f>
-        <v>7.2503293632281842</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H13" s="12">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>1.5735915849388864</v>
+      </c>
+      <c r="M13">
+        <f xml:space="preserve"> N13 - ($R$3*L13/SQRT($R$1))</f>
+        <v>3.4018133702230804</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>4.8571428571428568</v>
+      </c>
+      <c r="O13">
+        <f xml:space="preserve"> N13 + ($R$3*L13/SQRT($R$1))</f>
+        <v>6.3124723440626331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1887,98 +1994,125 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-      <c r="G14">
-        <f>_xlfn.STDEV.S(B14:E14)</f>
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="H14">
-        <f xml:space="preserve"> I14 - ($M$3*G14/SQRT($M$1))</f>
-        <v>0.74967063677181534</v>
-      </c>
-      <c r="I14">
-        <f>AVERAGE(B14:E14)</f>
-        <v>3</v>
-      </c>
-      <c r="J14">
-        <f xml:space="preserve"> I14 + ($M$3*G14/SQRT($M$1))</f>
-        <v>5.2503293632281842</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
+      <c r="F14" s="12">
+        <v>4</v>
+      </c>
+      <c r="G14" s="12">
+        <v>4</v>
+      </c>
+      <c r="H14" s="12">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1.3801311186847085</v>
+      </c>
+      <c r="M14">
+        <f xml:space="preserve"> N14 - ($R$3*L14/SQRT($R$1))</f>
+        <v>1.43787731704874</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="O14">
+        <f xml:space="preserve"> N14 + ($R$3*L14/SQRT($R$1))</f>
+        <v>3.9906941115226888</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-      <c r="G15">
-        <f>_xlfn.STDEV.S(B15:E15)</f>
-        <v>0.5</v>
-      </c>
-      <c r="H15">
-        <f xml:space="preserve"> I15 - ($M$3*G15/SQRT($M$1))</f>
-        <v>2.454388423679073</v>
-      </c>
-      <c r="I15">
-        <f>AVERAGE(B15:E15)</f>
-        <v>3.25</v>
-      </c>
-      <c r="J15">
-        <f xml:space="preserve"> I15 + ($M$3*G15/SQRT($M$1))</f>
-        <v>4.045611576320927</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E15" s="3">
+        <v>3</v>
+      </c>
+      <c r="F15" s="12">
+        <v>3</v>
+      </c>
+      <c r="G15" s="12">
+        <v>3</v>
+      </c>
+      <c r="H15" s="12">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>0.69006555934235381</v>
+      </c>
+      <c r="M15">
+        <f xml:space="preserve"> N15 - ($R$3*L15/SQRT($R$1))</f>
+        <v>2.2189386585243707</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="O15">
+        <f xml:space="preserve"> N15 + ($R$3*L15/SQRT($R$1))</f>
+        <v>3.4953470557613437</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="G16">
-        <f>_xlfn.STDEV.S(B16:E16)</f>
-        <v>0.57735026918962573</v>
-      </c>
-      <c r="H16">
-        <f xml:space="preserve"> I16 - ($M$3*G16/SQRT($M$1))</f>
-        <v>2.5813068844814602</v>
-      </c>
-      <c r="I16">
-        <f>AVERAGE(B16:E16)</f>
-        <v>3.5</v>
-      </c>
-      <c r="J16">
-        <f xml:space="preserve"> I16 + ($M$3*G16/SQRT($M$1))</f>
-        <v>4.4186931155185398</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="3">
+        <v>4</v>
+      </c>
+      <c r="F16" s="12">
+        <v>4</v>
+      </c>
+      <c r="G16" s="12">
+        <v>4</v>
+      </c>
+      <c r="H16" s="12">
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>1.2724180205607032</v>
+      </c>
+      <c r="M16">
+        <f xml:space="preserve"> N16 - ($R$3*L16/SQRT($R$1))</f>
+        <v>2.2517810321726044</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="O16">
+        <f xml:space="preserve"> N16 + ($R$3*L16/SQRT($R$1))</f>
+        <v>4.6053618249702524</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -1986,113 +2120,122 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>4</v>
-      </c>
-      <c r="G17">
-        <f>_xlfn.STDEV.S(B17:E17)</f>
-        <v>0.9574271077563381</v>
-      </c>
-      <c r="H17">
-        <f xml:space="preserve"> I17 - ($M$3*G17/SQRT($M$1))</f>
-        <v>1.726519819171187</v>
-      </c>
-      <c r="I17">
-        <f>AVERAGE(B17:E17)</f>
-        <v>3.25</v>
-      </c>
-      <c r="J17">
-        <f xml:space="preserve"> I17 + ($M$3*G17/SQRT($M$1))</f>
-        <v>4.7734801808288125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17" s="12">
+        <v>3</v>
+      </c>
+      <c r="G17" s="12">
+        <v>4</v>
+      </c>
+      <c r="H17" s="12">
+        <v>4</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>0.89973541084243702</v>
+      </c>
+      <c r="M17">
+        <f xml:space="preserve"> N17 - ($R$3*L17/SQRT($R$1))</f>
+        <v>2.0250263878140435</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="O17">
+        <f xml:space="preserve"> N17 + ($R$3*L17/SQRT($R$1))</f>
+        <v>3.6892593264716709</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G20">
-        <f xml:space="preserve"> AVERAGE(G2:G7)</f>
-        <v>0.88108248094035158</v>
-      </c>
-      <c r="H20">
-        <f xml:space="preserve"> AVERAGE(H2:H7)</f>
-        <v>1.473001156940587</v>
-      </c>
-      <c r="I20">
-        <f xml:space="preserve"> AVERAGE(I2:I7)</f>
-        <v>2.875</v>
-      </c>
-      <c r="J20">
-        <f xml:space="preserve"> AVERAGE(J2:J7)</f>
-        <v>4.2769988430594124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <f xml:space="preserve"> AVERAGE(L2:L7)</f>
+        <v>0.80330160187782507</v>
+      </c>
+      <c r="M20">
+        <f xml:space="preserve"> AVERAGE(M2:M7)</f>
+        <v>1.9475461193624124</v>
+      </c>
+      <c r="N20">
+        <f xml:space="preserve"> AVERAGE(N2:N7)</f>
+        <v>2.6904761904761902</v>
+      </c>
+      <c r="O20">
+        <f xml:space="preserve"> AVERAGE(O2:O7)</f>
+        <v>3.433406261589969</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G21">
-        <f xml:space="preserve"> AVERAGE(G8:G13)</f>
-        <v>1.3961624188737989</v>
-      </c>
-      <c r="H21">
-        <f xml:space="preserve"> AVERAGE(H8:H13)</f>
-        <v>2.6117273675728896</v>
-      </c>
-      <c r="I21">
-        <f xml:space="preserve"> AVERAGE(I8:I13)</f>
-        <v>4.833333333333333</v>
-      </c>
-      <c r="J21">
-        <f xml:space="preserve"> AVERAGE(J8:J13)</f>
-        <v>7.0549392990937774</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <f xml:space="preserve"> AVERAGE(L8:L13)</f>
+        <v>1.6809423640369763</v>
+      </c>
+      <c r="M21">
+        <f xml:space="preserve"> AVERAGE(M8:M13)</f>
+        <v>2.7072923633574875</v>
+      </c>
+      <c r="N21">
+        <f xml:space="preserve"> AVERAGE(N8:N13)</f>
+        <v>4.2619047619047619</v>
+      </c>
+      <c r="O21">
+        <f xml:space="preserve"> AVERAGE(O8:O13)</f>
+        <v>5.8165171604520358</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G22">
-        <f xml:space="preserve"> AVERAGE(G14:G16)</f>
-        <v>0.83052127718757374</v>
-      </c>
-      <c r="H22">
-        <f xml:space="preserve"> AVERAGE(H14:H16)</f>
-        <v>1.9284553149774493</v>
-      </c>
-      <c r="I22">
-        <f xml:space="preserve"> AVERAGE(I14:I16)</f>
-        <v>3.25</v>
-      </c>
-      <c r="J22">
-        <f xml:space="preserve"> AVERAGE(J14:J16)</f>
-        <v>4.571544685022551</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <f xml:space="preserve"> AVERAGE(L14:L16)</f>
+        <v>1.1142048995292553</v>
+      </c>
+      <c r="M22">
+        <f xml:space="preserve"> AVERAGE(M14:M16)</f>
+        <v>1.9695323359152386</v>
+      </c>
+      <c r="N22">
+        <f xml:space="preserve"> AVERAGE(N14:N16)</f>
+        <v>3</v>
+      </c>
+      <c r="O22">
+        <f xml:space="preserve"> AVERAGE(O14:O16)</f>
+        <v>4.0304676640847612</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G23">
-        <f xml:space="preserve"> AVERAGE(G2:G17)</f>
-        <v>1.0695287711377477</v>
-      </c>
-      <c r="H23">
-        <f xml:space="preserve"> AVERAGE(H2:H17)</f>
-        <v>2.0012660569490244</v>
-      </c>
-      <c r="I23">
-        <f xml:space="preserve"> AVERAGE(I2:I17)</f>
-        <v>3.703125</v>
-      </c>
-      <c r="J23">
-        <f xml:space="preserve"> AVERAGE(J2:J17)</f>
-        <v>5.4049839430509747</v>
+      <c r="L23">
+        <f xml:space="preserve"> AVERAGE(L2:L17)</f>
+        <v>1.196738369057438</v>
+      </c>
+      <c r="M23">
+        <f xml:space="preserve"> AVERAGE(M2:M17)</f>
+        <v>2.2414158932424475</v>
+      </c>
+      <c r="N23">
+        <f xml:space="preserve"> AVERAGE(N2:N17)</f>
+        <v>3.3482142857142856</v>
+      </c>
+      <c r="O23">
+        <f xml:space="preserve"> AVERAGE(O2:O17)</f>
+        <v>4.4550126781861241</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2271,32 +2414,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I3:I4 I5:I14 G3:G14" formulaRange="1"/>
+    <ignoredError sqref="L2:L17 N2:N17" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -2307,29 +2450,38 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
       <c r="G3">
-        <f>_xlfn.STDEV.S(B3:E3)</f>
-        <v>0.57735026918962573</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <f xml:space="preserve"> I3 - (PSSUQ!$M$3*G3/SQRT(PSSUQ!$M$1))</f>
-        <v>0.5813068844814604</v>
-      </c>
-      <c r="I3">
-        <f>AVERAGE(B3:E3)</f>
-        <v>1.5</v>
-      </c>
-      <c r="J3">
-        <f xml:space="preserve"> I3 + (PSSUQ!$M$3*G3/SQRT(PSSUQ!$M$1))</f>
-        <v>2.4186931155185398</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <f>_xlfn.STDEV.S(B3:H3)</f>
+        <v>1.6183471874253741</v>
+      </c>
+      <c r="O3">
+        <f xml:space="preserve"> P3 - (PSSUQ!$R$3*N3/SQRT(PSSUQ!$R$1))</f>
+        <v>0.93184991297861131</v>
+      </c>
+      <c r="P3">
+        <f>AVERAGE(B3:H3)</f>
+        <v>2.4285714285714284</v>
+      </c>
+      <c r="Q3">
+        <f xml:space="preserve"> P3 + (PSSUQ!$R$3*N3/SQRT(PSSUQ!$R$1))</f>
+        <v>3.9252929441642452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -2340,95 +2492,122 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
       <c r="G4">
-        <f>_xlfn.STDEV.S(B4:E4)</f>
-        <v>0.57735026918962573</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <f xml:space="preserve"> I4 - (PSSUQ!$M$3*G4/SQRT(PSSUQ!$M$1))</f>
-        <v>0.5813068844814604</v>
-      </c>
-      <c r="I4">
-        <f>AVERAGE(B4:E4)</f>
-        <v>1.5</v>
-      </c>
-      <c r="J4">
-        <f xml:space="preserve"> I4 + (PSSUQ!$M$3*G4/SQRT(PSSUQ!$M$1))</f>
-        <v>2.4186931155185398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N12" si="0">_xlfn.STDEV.S(B4:H4)</f>
+        <v>1.6183471874253741</v>
+      </c>
+      <c r="O4">
+        <f xml:space="preserve"> P4 - (PSSUQ!$R$3*N4/SQRT(PSSUQ!$R$1))</f>
+        <v>0.93184991297861131</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P12" si="1">AVERAGE(B4:H4)</f>
+        <v>2.4285714285714284</v>
+      </c>
+      <c r="Q4">
+        <f xml:space="preserve"> P4 + (PSSUQ!$R$3*N4/SQRT(PSSUQ!$R$1))</f>
+        <v>3.9252929441642452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
         <v>5</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>6</v>
       </c>
-      <c r="G5">
-        <f>_xlfn.STDEV.S(B5:E5)</f>
-        <v>1.2909944487358056</v>
-      </c>
-      <c r="H5">
-        <f xml:space="preserve"> I5 - (PSSUQ!$M$3*G5/SQRT(PSSUQ!$M$1))</f>
-        <v>2.4457397432394785</v>
-      </c>
-      <c r="I5">
-        <f>AVERAGE(B5:E5)</f>
-        <v>4.5</v>
-      </c>
-      <c r="J5">
-        <f xml:space="preserve"> I5 + (PSSUQ!$M$3*G5/SQRT(PSSUQ!$M$1))</f>
-        <v>6.5542602567605215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>1.7182493859684487</v>
+      </c>
+      <c r="O5">
+        <f xml:space="preserve"> P5 - (PSSUQ!$R$3*N5/SQRT(PSSUQ!$R$1))</f>
+        <v>1.839455789408424</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="Q5">
+        <f xml:space="preserve"> P5 + (PSSUQ!$R$3*N5/SQRT(PSSUQ!$R$1))</f>
+        <v>5.0176870677344327</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <v>6</v>
       </c>
-      <c r="G6">
-        <f>_xlfn.STDEV.S(B6:E6)</f>
-        <v>1.2909944487358056</v>
-      </c>
-      <c r="H6">
-        <f xml:space="preserve"> I6 - (PSSUQ!$M$3*G6/SQRT(PSSUQ!$M$1))</f>
-        <v>2.4457397432394785</v>
-      </c>
-      <c r="I6">
-        <f>AVERAGE(B6:E6)</f>
-        <v>4.5</v>
-      </c>
-      <c r="J6">
-        <f xml:space="preserve"> I6 + (PSSUQ!$M$3*G6/SQRT(PSSUQ!$M$1))</f>
-        <v>6.5542602567605215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>1.7182493859684487</v>
+      </c>
+      <c r="O6">
+        <f xml:space="preserve"> P6 - (PSSUQ!$R$3*N6/SQRT(PSSUQ!$R$1))</f>
+        <v>1.839455789408424</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="Q6">
+        <f xml:space="preserve"> P6 + (PSSUQ!$R$3*N6/SQRT(PSSUQ!$R$1))</f>
+        <v>5.0176870677344327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -2439,29 +2618,38 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
       <c r="G7">
-        <f>_xlfn.STDEV.S(B7:E7)</f>
-        <v>0.9574271077563381</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <f xml:space="preserve"> I7 - (PSSUQ!$M$3*G7/SQRT(PSSUQ!$M$1))</f>
-        <v>0.72651981917118702</v>
-      </c>
-      <c r="I7">
-        <f>AVERAGE(B7:E7)</f>
-        <v>2.25</v>
-      </c>
-      <c r="J7">
-        <f xml:space="preserve"> I7 + (PSSUQ!$M$3*G7/SQRT(PSSUQ!$M$1))</f>
-        <v>3.773480180828813</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0.75592894601845462</v>
+      </c>
+      <c r="O7">
+        <f xml:space="preserve"> P7 - (PSSUQ!$R$3*N7/SQRT(PSSUQ!$R$1))</f>
+        <v>1.5865966139585799</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="Q7">
+        <f xml:space="preserve"> P7 + (PSSUQ!$R$3*N7/SQRT(PSSUQ!$R$1))</f>
+        <v>2.9848319574699911</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -2469,98 +2657,125 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
         <v>5</v>
       </c>
-      <c r="G8">
-        <f>_xlfn.STDEV.S(B8:E8)</f>
-        <v>1.6329931618554521</v>
-      </c>
-      <c r="H8">
-        <f xml:space="preserve"> I8 - (PSSUQ!$M$3*G8/SQRT(PSSUQ!$M$1))</f>
-        <v>0.40154347274977731</v>
-      </c>
-      <c r="I8">
-        <f>AVERAGE(B8:E8)</f>
-        <v>3</v>
-      </c>
-      <c r="J8">
-        <f xml:space="preserve"> I8 + (PSSUQ!$M$3*G8/SQRT(PSSUQ!$M$1))</f>
-        <v>5.5984565272502227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>1.2535663410560176</v>
+      </c>
+      <c r="O8">
+        <f xml:space="preserve"> P8 - (PSSUQ!$R$3*N8/SQRT(PSSUQ!$R$1))</f>
+        <v>1.554930213525453</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="Q8">
+        <f xml:space="preserve"> P8 + (PSSUQ!$R$3*N8/SQRT(PSSUQ!$R$1))</f>
+        <v>3.8736412150459758</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
         <v>5</v>
       </c>
-      <c r="G9">
-        <f>_xlfn.STDEV.S(B9:E9)</f>
-        <v>1.2583057392117916</v>
-      </c>
-      <c r="H9">
-        <f xml:space="preserve"> I9 - (PSSUQ!$M$3*G9/SQRT(PSSUQ!$M$1))</f>
-        <v>1.2477547746640738</v>
-      </c>
-      <c r="I9">
-        <f>AVERAGE(B9:E9)</f>
-        <v>3.25</v>
-      </c>
-      <c r="J9">
-        <f xml:space="preserve"> I9 + (PSSUQ!$M$3*G9/SQRT(PSSUQ!$M$1))</f>
-        <v>5.2522452253359262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>1.2535663410560176</v>
+      </c>
+      <c r="O9">
+        <f xml:space="preserve"> P9 - (PSSUQ!$R$3*N9/SQRT(PSSUQ!$R$1))</f>
+        <v>1.554930213525453</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="Q9">
+        <f xml:space="preserve"> P9 + (PSSUQ!$R$3*N9/SQRT(PSSUQ!$R$1))</f>
+        <v>3.8736412150459758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
         <v>5</v>
       </c>
-      <c r="G10">
-        <f>_xlfn.STDEV.S(B10:E10)</f>
-        <v>1.2583057392117916</v>
-      </c>
-      <c r="H10">
-        <f xml:space="preserve"> I10 - (PSSUQ!$M$3*G10/SQRT(PSSUQ!$M$1))</f>
-        <v>1.2477547746640738</v>
-      </c>
-      <c r="I10">
-        <f>AVERAGE(B10:E10)</f>
-        <v>3.25</v>
-      </c>
-      <c r="J10">
-        <f xml:space="preserve"> I10 + (PSSUQ!$M$3*G10/SQRT(PSSUQ!$M$1))</f>
-        <v>5.2522452253359262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>1.2724180205607036</v>
+      </c>
+      <c r="O10">
+        <f xml:space="preserve"> P10 - (PSSUQ!$R$3*N10/SQRT(PSSUQ!$R$1))</f>
+        <v>1.394638175029747</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="Q10">
+        <f xml:space="preserve"> P10 + (PSSUQ!$R$3*N10/SQRT(PSSUQ!$R$1))</f>
+        <v>3.7482189678273965</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -2568,32 +2783,41 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
         <v>5</v>
       </c>
-      <c r="G11">
-        <f>_xlfn.STDEV.S(B11:E11)</f>
-        <v>1.8257418583505538</v>
-      </c>
-      <c r="H11">
-        <f xml:space="preserve"> I11 - (PSSUQ!$M$3*G11/SQRT(PSSUQ!$M$1))</f>
-        <v>9.4837284245233633E-2</v>
-      </c>
-      <c r="I11">
-        <f>AVERAGE(B11:E11)</f>
-        <v>3</v>
-      </c>
-      <c r="J11">
-        <f xml:space="preserve"> I11 + (PSSUQ!$M$3*G11/SQRT(PSSUQ!$M$1))</f>
-        <v>5.9051627157547664</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>1.511857892036909</v>
+      </c>
+      <c r="O11">
+        <f xml:space="preserve"> P11 - (PSSUQ!$R$3*N11/SQRT(PSSUQ!$R$1))</f>
+        <v>1.0303360850600169</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>2.4285714285714284</v>
+      </c>
+      <c r="Q11">
+        <f xml:space="preserve"> P11 + (PSSUQ!$R$3*N11/SQRT(PSSUQ!$R$1))</f>
+        <v>3.8268067720828398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -2607,27 +2831,39 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
       </c>
       <c r="G12">
-        <f>_xlfn.STDEV.S(B12:E12)</f>
-        <v>0.81649658092772603</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <f xml:space="preserve"> I12 - (PSSUQ!$M$3*G12/SQRT(PSSUQ!$M$1))</f>
-        <v>0.70077173637488865</v>
-      </c>
-      <c r="I12">
-        <f>AVERAGE(B12:E12)</f>
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <f xml:space="preserve"> I12 + (PSSUQ!$M$3*G12/SQRT(PSSUQ!$M$1))</f>
-        <v>3.2992282636251113</v>
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>0.95118973121134198</v>
+      </c>
+      <c r="O12">
+        <f xml:space="preserve"> P12 - (PSSUQ!$R$3*N12/SQRT(PSSUQ!$R$1))</f>
+        <v>1.4060105069596958</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="Q12">
+        <f xml:space="preserve"> P12 + (PSSUQ!$R$3*N12/SQRT(PSSUQ!$R$1))</f>
+        <v>3.1654180644688754</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="N3:N12 P3:P12" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -2635,8 +2871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2741,10 +2977,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2759,19 +2995,19 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -2783,7 +3019,7 @@
         <v>2</v>
       </c>
       <c r="P2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -2792,22 +3028,22 @@
         <v>1</v>
       </c>
       <c r="S2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W2">
         <v>2</v>
       </c>
       <c r="X2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y2">
         <v>1</v>
@@ -2825,7 +3061,7 @@
         <v>1</v>
       </c>
       <c r="AD2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE2">
         <v>1</v>
@@ -2845,31 +3081,31 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -2884,28 +3120,28 @@
         <v>2</v>
       </c>
       <c r="R3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
         <v>2</v>
       </c>
       <c r="U3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W3">
         <v>2</v>
       </c>
       <c r="X3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z3">
         <v>2</v>
@@ -2914,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="AB3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC3">
         <v>2</v>
@@ -2923,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="AE3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
@@ -2931,94 +3167,94 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N4">
         <v>2</v>
       </c>
       <c r="O4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S4">
         <v>3</v>
       </c>
       <c r="T4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y4">
         <v>3</v>
       </c>
       <c r="Z4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC4">
         <v>2</v>
       </c>
       <c r="AD4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
@@ -3026,101 +3262,380 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5">
+        <v>3</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5">
+        <v>2</v>
+      </c>
+      <c r="X5">
+        <v>2</v>
+      </c>
+      <c r="Y5">
+        <v>3</v>
+      </c>
+      <c r="Z5">
+        <v>2</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>2</v>
+      </c>
+      <c r="AC5">
+        <v>2</v>
+      </c>
+      <c r="AD5">
+        <v>3</v>
+      </c>
+      <c r="AE5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="J5">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
         <v>5</v>
       </c>
-      <c r="K5">
-        <v>4</v>
-      </c>
-      <c r="L5">
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6">
+        <v>3</v>
+      </c>
+      <c r="V6">
+        <v>3</v>
+      </c>
+      <c r="W6">
+        <v>2</v>
+      </c>
+      <c r="X6">
+        <v>2</v>
+      </c>
+      <c r="Y6">
+        <v>3</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6">
+        <v>2</v>
+      </c>
+      <c r="AB6">
+        <v>3</v>
+      </c>
+      <c r="AC6">
+        <v>2</v>
+      </c>
+      <c r="AD6">
+        <v>3</v>
+      </c>
+      <c r="AE6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="M5">
-        <v>4</v>
-      </c>
-      <c r="N5">
-        <v>4</v>
-      </c>
-      <c r="O5">
-        <v>4</v>
-      </c>
-      <c r="P5">
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
         <v>5</v>
       </c>
-      <c r="Q5">
-        <v>3</v>
-      </c>
-      <c r="R5">
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+      <c r="T7">
+        <v>3</v>
+      </c>
+      <c r="U7">
+        <v>4</v>
+      </c>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>3</v>
+      </c>
+      <c r="X7">
+        <v>4</v>
+      </c>
+      <c r="Y7">
+        <v>3</v>
+      </c>
+      <c r="Z7">
+        <v>3</v>
+      </c>
+      <c r="AA7">
+        <v>3</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
+      </c>
+      <c r="AC7">
+        <v>3</v>
+      </c>
+      <c r="AD7">
+        <v>4</v>
+      </c>
+      <c r="AE7">
         <v>5</v>
       </c>
-      <c r="S5">
-        <v>3</v>
-      </c>
-      <c r="T5">
-        <v>3</v>
-      </c>
-      <c r="U5">
-        <v>4</v>
-      </c>
-      <c r="V5">
-        <v>3</v>
-      </c>
-      <c r="W5">
-        <v>3</v>
-      </c>
-      <c r="X5">
-        <v>4</v>
-      </c>
-      <c r="Y5">
-        <v>3</v>
-      </c>
-      <c r="Z5">
-        <v>4</v>
-      </c>
-      <c r="AA5">
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="AB5">
-        <v>3</v>
-      </c>
-      <c r="AC5">
-        <v>3</v>
-      </c>
-      <c r="AD5">
-        <v>4</v>
-      </c>
-      <c r="AE5">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8">
+        <v>5</v>
+      </c>
+      <c r="T8">
+        <v>3</v>
+      </c>
+      <c r="U8">
+        <v>5</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+      <c r="W8">
+        <v>3</v>
+      </c>
+      <c r="X8">
+        <v>4</v>
+      </c>
+      <c r="Y8">
+        <v>5</v>
+      </c>
+      <c r="Z8">
+        <v>4</v>
+      </c>
+      <c r="AA8">
+        <v>5</v>
+      </c>
+      <c r="AB8">
+        <v>4</v>
+      </c>
+      <c r="AC8">
+        <v>3</v>
+      </c>
+      <c r="AD8">
+        <v>4</v>
+      </c>
+      <c r="AE8">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="J12" s="8"/>
@@ -3139,124 +3654,124 @@
         <v>74</v>
       </c>
       <c r="B15">
-        <f>AVERAGE(B2:B6)</f>
-        <v>2.75</v>
+        <f>AVERAGE(B2:B8)</f>
+        <v>2.2857142857142856</v>
       </c>
       <c r="C15">
-        <f>AVERAGE(C2:C6)</f>
-        <v>2.75</v>
+        <f>AVERAGE(C2:C8)</f>
+        <v>2.2857142857142856</v>
       </c>
       <c r="D15">
-        <f>AVERAGE(D2:D6)</f>
-        <v>2.5</v>
+        <f>AVERAGE(D2:D8)</f>
+        <v>2.7142857142857144</v>
       </c>
       <c r="E15">
-        <f>AVERAGE(E2:E6)</f>
-        <v>2.25</v>
+        <f>AVERAGE(E2:E8)</f>
+        <v>2</v>
       </c>
       <c r="F15">
-        <f>AVERAGE(F2:F6)</f>
-        <v>2.75</v>
+        <f>AVERAGE(F2:F8)</f>
+        <v>2.4285714285714284</v>
       </c>
       <c r="G15">
-        <f>AVERAGE(G2:G6)</f>
-        <v>2.25</v>
+        <f>AVERAGE(G2:G8)</f>
+        <v>2.5714285714285716</v>
       </c>
       <c r="H15">
-        <f>AVERAGE(H2:H6)</f>
-        <v>3.25</v>
+        <f>AVERAGE(H2:H8)</f>
+        <v>2.5714285714285716</v>
       </c>
       <c r="I15">
-        <f>AVERAGE(I2:I6)</f>
-        <v>4</v>
+        <f>AVERAGE(I2:I8)</f>
+        <v>2.8571428571428572</v>
       </c>
       <c r="J15">
-        <f>AVERAGE(J2:J6)</f>
-        <v>3.5</v>
+        <f>AVERAGE(J2:J8)</f>
+        <v>3</v>
       </c>
       <c r="K15">
-        <f>AVERAGE(K2:K5)</f>
-        <v>4</v>
+        <f>AVERAGE(K2:K8)</f>
+        <v>3</v>
       </c>
       <c r="L15">
-        <f>AVERAGE(L2:L6)</f>
-        <v>4.5</v>
+        <f>AVERAGE(L2:L8)</f>
+        <v>3.1428571428571428</v>
       </c>
       <c r="M15">
-        <f>AVERAGE(M2:M6)</f>
-        <v>2.75</v>
+        <f>AVERAGE(M2:M8)</f>
+        <v>2.5714285714285716</v>
       </c>
       <c r="N15">
-        <f>AVERAGE(N2:N6)</f>
-        <v>2.5</v>
+        <f>AVERAGE(N2:N8)</f>
+        <v>2.4285714285714284</v>
       </c>
       <c r="O15">
-        <f>AVERAGE(O2:O6)</f>
-        <v>2.75</v>
+        <f>AVERAGE(O2:O8)</f>
+        <v>2.7142857142857144</v>
       </c>
       <c r="P15">
-        <f>AVERAGE(P2:P6)</f>
-        <v>3</v>
+        <f>AVERAGE(P2:P8)</f>
+        <v>2.8571428571428572</v>
       </c>
       <c r="Q15">
-        <f>AVERAGE(Q2:Q6)</f>
-        <v>2.25</v>
+        <f>AVERAGE(Q2:Q8)</f>
+        <v>2.2857142857142856</v>
       </c>
       <c r="R15">
-        <f>AVERAGE(R2:R5)</f>
-        <v>3.25</v>
+        <f>AVERAGE(R2:R8)</f>
+        <v>2.7142857142857144</v>
       </c>
       <c r="S15">
-        <f>AVERAGE(S2:S5)</f>
-        <v>2.75</v>
+        <f>AVERAGE(S2:S8)</f>
+        <v>2.8571428571428572</v>
       </c>
       <c r="T15">
-        <f>AVERAGE(T2:T5)</f>
-        <v>2.5</v>
+        <f>AVERAGE(T2:T8)</f>
+        <v>2.1428571428571428</v>
       </c>
       <c r="U15">
-        <f>AVERAGE(U2:U5)</f>
-        <v>3</v>
+        <f>AVERAGE(U2:U8)</f>
+        <v>2.8571428571428572</v>
       </c>
       <c r="V15">
-        <f>AVERAGE(V2:V5)</f>
-        <v>2.75</v>
+        <f>AVERAGE(V2:V8)</f>
+        <v>2.7142857142857144</v>
       </c>
       <c r="W15">
-        <f>AVERAGE(W2:W5)</f>
-        <v>2.5</v>
+        <f>AVERAGE(W2:W8)</f>
+        <v>2.2857142857142856</v>
       </c>
       <c r="X15">
-        <f>AVERAGE(X2:X5)</f>
-        <v>3</v>
+        <f>AVERAGE(X2:X8)</f>
+        <v>2.2857142857142856</v>
       </c>
       <c r="Y15">
-        <f>AVERAGE(Y2:Y5)</f>
-        <v>2.5</v>
+        <f>AVERAGE(Y2:Y8)</f>
+        <v>2.7142857142857144</v>
       </c>
       <c r="Z15">
-        <f>AVERAGE(Z2:Z5)</f>
-        <v>2.5</v>
+        <f>AVERAGE(Z2:Z8)</f>
+        <v>2.2857142857142856</v>
       </c>
       <c r="AA15">
-        <f>AVERAGE(AA2:AA5)</f>
-        <v>2.5</v>
+        <f>AVERAGE(AA2:AA8)</f>
+        <v>2</v>
       </c>
       <c r="AB15">
-        <f>AVERAGE(AB2:AB5)</f>
-        <v>2.25</v>
+        <f>AVERAGE(AB2:AB8)</f>
+        <v>2.2857142857142856</v>
       </c>
       <c r="AC15">
-        <f>AVERAGE(AC2:AC5)</f>
-        <v>2</v>
+        <f>AVERAGE(AC2:AC8)</f>
+        <v>2.1428571428571428</v>
       </c>
       <c r="AD15">
-        <f>AVERAGE(AD2:AD5)</f>
-        <v>3</v>
+        <f>AVERAGE(AD2:AD8)</f>
+        <v>2.7142857142857144</v>
       </c>
       <c r="AE15">
-        <f>AVERAGE(AE2:AE5)</f>
-        <v>2.75</v>
+        <f>AVERAGE(AE2:AE8)</f>
+        <v>2.7142857142857144</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
@@ -3265,43 +3780,43 @@
       </c>
       <c r="C16">
         <f>AVERAGE(B15:D15)</f>
-        <v>2.6666666666666665</v>
+        <v>2.4285714285714284</v>
       </c>
       <c r="F16">
         <f>AVERAGE(E15:G15)</f>
-        <v>2.4166666666666665</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="I16">
         <f>AVERAGE(H15:J15)</f>
-        <v>3.5833333333333335</v>
+        <v>2.8095238095238098</v>
       </c>
       <c r="L16">
         <f>AVERAGE(K15:M15)</f>
-        <v>3.75</v>
+        <v>2.9047619047619047</v>
       </c>
       <c r="O16">
         <f>AVERAGE(N15:P15)</f>
-        <v>2.75</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="R16">
         <f>AVERAGE(Q15:S15)</f>
-        <v>2.75</v>
+        <v>2.6190476190476191</v>
       </c>
       <c r="U16">
         <f>AVERAGE(T15:V15)</f>
-        <v>2.75</v>
+        <v>2.5714285714285716</v>
       </c>
       <c r="X16">
         <f>AVERAGE(W15:Y15)</f>
-        <v>2.6666666666666665</v>
+        <v>2.4285714285714284</v>
       </c>
       <c r="AA16">
         <f>AVERAGE(Z15:AB15)</f>
-        <v>2.4166666666666665</v>
+        <v>2.1904761904761902</v>
       </c>
       <c r="AD16">
         <f>AVERAGE(AC15:AE15)</f>
-        <v>2.5833333333333335</v>
+        <v>2.5238095238095242</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
@@ -3310,43 +3825,43 @@
       </c>
       <c r="C18">
         <f>_xlfn.STDEV.S(B2:D5)</f>
-        <v>1.1547005383792517</v>
+        <v>0.65133894727892949</v>
       </c>
       <c r="F18">
         <f>_xlfn.STDEV.S(E2:G5)</f>
-        <v>1.083624669450832</v>
+        <v>0.66855792342152154</v>
       </c>
       <c r="I18">
         <f>_xlfn.STDEV.S(H2:J5)</f>
-        <v>1.0836246694508314</v>
+        <v>0.7177405625652733</v>
       </c>
       <c r="L18">
         <f>_xlfn.STDEV.S(K2:M5)</f>
-        <v>1.1381803659589922</v>
+        <v>0.99620491989562177</v>
       </c>
       <c r="O18">
         <f>_xlfn.STDEV.S(N2:P5)</f>
-        <v>1.0552897060221726</v>
+        <v>0.42640143271122088</v>
       </c>
       <c r="R18">
         <f>_xlfn.STDEV.S(Q2:S5)</f>
-        <v>1.1381803659589922</v>
+        <v>0.66855792342152132</v>
       </c>
       <c r="U18">
         <f>_xlfn.STDEV.S(T2:V5)</f>
-        <v>0.75377836144440913</v>
+        <v>0.79296146109875898</v>
       </c>
       <c r="X18">
         <f>_xlfn.STDEV.S(W2:Y5)</f>
-        <v>0.88762536459859476</v>
+        <v>0.7177405625652733</v>
       </c>
       <c r="AA18">
         <f>_xlfn.STDEV.S(Z2:AB5)</f>
-        <v>1.3113721705515067</v>
+        <v>0.51492865054443737</v>
       </c>
       <c r="AD18">
-        <f>_xlfn.STDEV.S(AC2:AE5)</f>
-        <v>1.2401124093721456</v>
+        <f>_xlfn.STDEV.S(AC2:AD5)</f>
+        <v>0.64086994446165568</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
@@ -3355,43 +3870,43 @@
       </c>
       <c r="C19">
         <f>_xlfn.SKEW.P(B2:D5)</f>
-        <v>-5.4820244468683776E-2</v>
+        <v>0.38180177416060584</v>
       </c>
       <c r="F19">
         <f>_xlfn.SKEW.P(E2:G5)</f>
-        <v>-1.0364120372929493E-3</v>
+        <v>0.63991159634642314</v>
       </c>
       <c r="I19">
         <f>_xlfn.SKEW.P(H2:J5)</f>
-        <v>1.0364120372931367E-3</v>
+        <v>0.22826882356360798</v>
       </c>
       <c r="L19">
         <f>_xlfn.SKEW.P(K2:M5)</f>
-        <v>-1.0384080585720157</v>
+        <v>0.74298192299266852</v>
       </c>
       <c r="O19">
         <f>_xlfn.SKEW.P(N2:P5)</f>
-        <v>0.99984274022926467</v>
+        <v>0</v>
       </c>
       <c r="R19">
         <f>_xlfn.SKEW.P(Q2:S5)</f>
-        <v>0.12074512308976931</v>
+        <v>7.5024118192338854E-2</v>
       </c>
       <c r="U19">
         <f>_xlfn.SKEW.P(T2:V5)</f>
-        <v>0.41569219381653061</v>
+        <v>0.14018086215550785</v>
       </c>
       <c r="X19">
         <f>_xlfn.SKEW.P(W2:Y5)</f>
-        <v>-0.12068685239272803</v>
+        <v>0.22826882356360798</v>
       </c>
       <c r="AA19">
         <f>_xlfn.SKEW.P(Z2:AB5)</f>
-        <v>0.44150757731980517</v>
+        <v>0.33806170189140611</v>
       </c>
       <c r="AD19">
-        <f>_xlfn.SKEW.P(AC2:AE5)</f>
-        <v>0.54835161402016885</v>
+        <f>_xlfn.SKEW.P(AC2:AD5)</f>
+        <v>5.4395064536628346E-2</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
@@ -3400,43 +3915,43 @@
       </c>
       <c r="C20">
         <f>KURT(B2:D5)</f>
-        <v>-1.4727272727272736</v>
+        <v>-0.3367346938775535</v>
       </c>
       <c r="F20">
         <f>KURT(E2:G5)</f>
-        <v>-1.1526992715920934</v>
+        <v>-0.18960068945705233</v>
       </c>
       <c r="I20">
         <f>KURT(H2:J5)</f>
-        <v>-1.1526992715920912</v>
+        <v>-0.68512110726643582</v>
       </c>
       <c r="L20">
         <f>KURT(K2:M5)</f>
-        <v>2.1153585718682679</v>
+        <v>-1.3845347007750419E-2</v>
       </c>
       <c r="O20">
         <f>KURT(N2:P5)</f>
-        <v>0.12583645703179247</v>
+        <v>5.5</v>
       </c>
       <c r="R20">
         <f>KURT(Q2:S5)</f>
-        <v>0.42523853493382546</v>
+        <v>-0.18960068945705588</v>
       </c>
       <c r="U20">
         <f>KURT(T2:V5)</f>
-        <v>-0.86826666666666874</v>
+        <v>-1.2607925678618086</v>
       </c>
       <c r="X20">
         <f>KURT(W2:Y5)</f>
-        <v>-0.25384615384615472</v>
+        <v>-0.68512110726643538</v>
       </c>
       <c r="AA20">
         <f>KURT(Z2:AB5)</f>
-        <v>-0.43906926196898954</v>
+        <v>-2.2628571428571433</v>
       </c>
       <c r="AD20">
-        <f>KURT(AC2:AE5)</f>
-        <v>-0.34402193695551775</v>
+        <f>KURT(AC2:AD5)</f>
+        <v>0.7410207939508533</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
@@ -3489,39 +4004,39 @@
       </c>
       <c r="C24">
         <f>CORREL(E$15:G$15,$B$15:$D$15)</f>
-        <v>0.5</v>
+        <v>0.69337524528153671</v>
       </c>
       <c r="D24">
         <f>CORREL($H$15:$J$15,$B$15:$D$15)</f>
-        <v>0.18898223650461363</v>
+        <v>0.7559289460184544</v>
       </c>
       <c r="E24">
         <f>CORREL($K15:$M15,$B$15:$D$15)</f>
-        <v>0.96076892283052284</v>
+        <v>-0.97072534339415084</v>
       </c>
       <c r="F24">
         <f>CORREL($N15:$P15,$B$15:$D$15)</f>
-        <v>-0.8660254037844386</v>
+        <v>0.75592894601845428</v>
       </c>
       <c r="G24">
         <f>CORREL($Q$15:$S$15,$B$15:$D$15)</f>
-        <v>0</v>
+        <v>0.69337524528153627</v>
       </c>
       <c r="H24">
         <f>CORREL($T$15:$V$15,$B$15:$D$15)</f>
-        <v>0</v>
+        <v>0.32732683535398877</v>
       </c>
       <c r="I24">
         <f>CORREL($W$15:$Y$15,$B$15:$D$15)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <f>CORREL($Z$15:$AB$15,$B$15:$D$15)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K24">
         <f>CORREL($AC$15:$AE$15,$B$15:$D$15)</f>
-        <v>-0.27735009811261452</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
@@ -3536,35 +4051,35 @@
       </c>
       <c r="D25">
         <f>CORREL($H$15:$J$15,$E$15:$G$15)</f>
-        <v>0.94491118252306794</v>
+        <v>0.99587059488582252</v>
       </c>
       <c r="E25">
         <f>CORREL($K15:$M15,$E$15:$G$15)</f>
-        <v>0.72057669212289222</v>
+        <v>-0.50000000000000056</v>
       </c>
       <c r="F25">
         <f>CORREL($N15:$P15,$E$15:$G$15)</f>
-        <v>0</v>
+        <v>0.99587059488582241</v>
       </c>
       <c r="G25">
         <f>CORREL($Q$15:$S$15,$E$15:$G$15)</f>
-        <v>0.8660254037844386</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="H25">
         <f>CORREL($T$15:$V$15,$E$15:$G$15)</f>
-        <v>0.8660254037844386</v>
+        <v>0.90784129900320343</v>
       </c>
       <c r="I25">
         <f>CORREL($W$15:$Y$15,$E$15:$G$15)</f>
-        <v>1.0000000000000002</v>
+        <v>0.69337524528153671</v>
       </c>
       <c r="J25">
         <f>CORREL($Z$15:$AB$15,$E$15:$G$15)</f>
-        <v>0.5</v>
+        <v>-0.27735009811261391</v>
       </c>
       <c r="K25">
         <f>CORREL($AC$15:$AE$15,$E$15:$G$15)</f>
-        <v>0.69337524528153627</v>
+        <v>0.97072534339415062</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
@@ -3573,42 +4088,42 @@
       </c>
       <c r="B26">
         <f>CORREL($H$15:$J$15,$B$15:$D$15)</f>
-        <v>0.18898223650461363</v>
+        <v>0.7559289460184544</v>
       </c>
       <c r="C26">
         <f>CORREL($H$15:$J$15,$E$15:$G$15)</f>
-        <v>0.94491118252306794</v>
+        <v>0.99587059488582252</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
         <f>CORREL($K15:$M15,$H$15:$J$15)</f>
-        <v>0.45392064950160188</v>
+        <v>-0.57655666019705509</v>
       </c>
       <c r="F26">
         <f>CORREL($N15:$P15,$H$15:$J$15)</f>
-        <v>0.3273268353539886</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <f>CORREL($Q$15:$S$15,$H$15:$J$15)</f>
-        <v>0.98198050606196585</v>
+        <v>0.99587059488582241</v>
       </c>
       <c r="H26">
         <f>CORREL($T$15:$V$15,$H$15:$J$15)</f>
-        <v>0.98198050606196585</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="I26">
         <f>CORREL($W$15:$Y$15,$H$15:$J$15)</f>
-        <v>0.94491118252306794</v>
+        <v>0.7559289460184544</v>
       </c>
       <c r="J26">
         <f>CORREL($Z$15:$AB$15,$H$15:$J$15)</f>
-        <v>0.18898223650461363</v>
+        <v>-0.18898223650461363</v>
       </c>
       <c r="K26">
         <f>CORREL($AC$15:$AE$15,$H$15:$J$15)</f>
-        <v>0.89104211121363075</v>
+        <v>0.94491118252306805</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -3617,42 +4132,42 @@
       </c>
       <c r="B27">
         <f>CORREL($K15:$M15,$B$15:$D$15)</f>
-        <v>0.96076892283052284</v>
+        <v>-0.97072534339415084</v>
       </c>
       <c r="C27">
         <f>CORREL($K15:$M15,$E$15:$G$15)</f>
-        <v>0.72057669212289222</v>
+        <v>-0.50000000000000056</v>
       </c>
       <c r="D27">
         <f>CORREL($K15:$M15,$H$15:$J$15)</f>
-        <v>0.45392064950160188</v>
+        <v>-0.57655666019705509</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27">
         <f>CORREL($N15:$P15,$K$15:$M$15)</f>
-        <v>-0.69337524528153638</v>
+        <v>-0.57655666019705476</v>
       </c>
       <c r="G27">
         <f>CORREL($Q$15:$S$15,$K$15:$M$15)</f>
-        <v>0.27735009811261452</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="H27">
         <f>CORREL($T$15:$V$15,$K$15:$M$15)</f>
-        <v>0.27735009811261452</v>
+        <v>-9.078412990032049E-2</v>
       </c>
       <c r="I27">
         <f>CORREL($W$15:$Y$15,$K$15:$M$15)</f>
-        <v>0.72057669212289222</v>
+        <v>-0.97072534339415084</v>
       </c>
       <c r="J27">
         <f>CORREL($Z$15:$AB$15,$K$15:$M$15)</f>
-        <v>0.96076892283052284</v>
+        <v>-0.69337524528153649</v>
       </c>
       <c r="K27">
         <f>CORREL($AC$15:$AE$15,$K$15:$M$15)</f>
-        <v>0</v>
+        <v>-0.27735009811261463</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
@@ -3661,42 +4176,42 @@
       </c>
       <c r="B28">
         <f>CORREL($N15:$P15,$B$15:$D$15)</f>
-        <v>-0.8660254037844386</v>
+        <v>0.75592894601845428</v>
       </c>
       <c r="C28">
         <f>CORREL($N15:$P15,$E$15:$G$15)</f>
-        <v>0</v>
+        <v>0.99587059488582241</v>
       </c>
       <c r="D28">
         <f>CORREL($N15:$P15,$H$15:$J$15)</f>
-        <v>0.3273268353539886</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <f>CORREL($N15:$P15,$K$15:$M$15)</f>
-        <v>-0.69337524528153638</v>
+        <v>-0.57655666019705476</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
       <c r="G28">
         <f>CORREL($Q$15:$S$15,$N$15:$P$15)</f>
-        <v>0.5</v>
+        <v>0.99587059488582252</v>
       </c>
       <c r="H28">
         <f>CORREL($T$15:$V$15,$N$15:$P$15)</f>
-        <v>0.5</v>
+        <v>0.86602540378443893</v>
       </c>
       <c r="I28">
         <f>CORREL($W$15:$Y$15,$N$15:$P$15)</f>
-        <v>0</v>
+        <v>0.75592894601845428</v>
       </c>
       <c r="J28">
         <f>CORREL($Z$15:$AB$15,$N$15:$P$15)</f>
-        <v>-0.8660254037844386</v>
+        <v>-0.18898223650461399</v>
       </c>
       <c r="K28">
         <f>CORREL($AC$15:$AE$15,$N$15:$P$15)</f>
-        <v>0.7205766921228921</v>
+        <v>0.94491118252306816</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
@@ -3705,42 +4220,42 @@
       </c>
       <c r="B29">
         <f>CORREL($Q$15:$S$15,$B$15:$D$15)</f>
-        <v>0</v>
+        <v>0.69337524528153627</v>
       </c>
       <c r="C29">
         <f>CORREL($Q$15:$S$15,$E$15:$G$15)</f>
-        <v>0.8660254037844386</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="D29">
         <f>CORREL($Q$15:$S$15,$H$15:$J$15)</f>
-        <v>0.98198050606196585</v>
+        <v>0.99587059488582241</v>
       </c>
       <c r="E29">
         <f>CORREL($Q$15:$S$15,$K$15:$M$15)</f>
-        <v>0.27735009811261452</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="F29">
         <f>CORREL($Q$15:$S$15,$N$15:$P$15)</f>
-        <v>0.5</v>
+        <v>0.99587059488582252</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29">
         <f>CORREL($T$15:$V$15,$Q$15:$S$15)</f>
-        <v>1</v>
+        <v>0.90784129900320376</v>
       </c>
       <c r="I29">
         <f>CORREL($W$15:$Y$15,$Q$15:$S$15)</f>
-        <v>0.8660254037844386</v>
+        <v>0.69337524528153627</v>
       </c>
       <c r="J29">
         <f>CORREL($Z$15:$AB$15,$Q$15:$S$15)</f>
-        <v>0</v>
+        <v>-0.27735009811261474</v>
       </c>
       <c r="K29">
         <f>CORREL($AC$15:$AE$15,$Q$15:$S$15)</f>
-        <v>0.96076892283052273</v>
+        <v>0.97072534339415084</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
@@ -3749,42 +4264,42 @@
       </c>
       <c r="B30">
         <f>CORREL($T$15:$V$15,$B$15:$D$15)</f>
-        <v>0</v>
+        <v>0.32732683535398877</v>
       </c>
       <c r="C30">
         <f>CORREL($T$15:$V$15,$E$15:$G$15)</f>
-        <v>0.8660254037844386</v>
+        <v>0.90784129900320343</v>
       </c>
       <c r="D30">
         <f>CORREL($T$15:$V$15,$H$15:$J$15)</f>
-        <v>0.98198050606196585</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="E30">
         <f>CORREL($T$15:$V$15,$K$15:$M$15)</f>
-        <v>0.27735009811261452</v>
+        <v>-9.078412990032049E-2</v>
       </c>
       <c r="F30">
         <f>CORREL($T$15:$V$15,$N$15:$P$15)</f>
-        <v>0.5</v>
+        <v>0.86602540378443893</v>
       </c>
       <c r="G30">
         <f>CORREL($T$15:$V$15,$Q$15:$S$15)</f>
-        <v>1</v>
+        <v>0.90784129900320376</v>
       </c>
       <c r="H30">
         <v>1</v>
       </c>
       <c r="I30">
         <f>CORREL($W$15:$Y$15,$T$15:$V$15)</f>
-        <v>0.8660254037844386</v>
+        <v>0.32732683535398877</v>
       </c>
       <c r="J30">
         <f>CORREL($Z$15:$AB$15,$Q$15:$S$15)</f>
-        <v>0</v>
+        <v>-0.27735009811261474</v>
       </c>
       <c r="K30">
         <f>CORREL($AC$15:$AE$15,$Q$15:$S$15)</f>
-        <v>0.96076892283052273</v>
+        <v>0.97072534339415084</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
@@ -3793,31 +4308,31 @@
       </c>
       <c r="B31">
         <f>CORREL($W$15:$Y$15,$B$15:$D$15)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C31">
         <f>CORREL($W$15:$Y$15,$E$15:$G$15)</f>
-        <v>1.0000000000000002</v>
+        <v>0.69337524528153671</v>
       </c>
       <c r="D31">
         <f>CORREL($W$15:$Y$15,$H$15:$J$15)</f>
-        <v>0.94491118252306794</v>
+        <v>0.7559289460184544</v>
       </c>
       <c r="E31">
         <f>CORREL($W$15:$Y$15,$K$15:$M$15)</f>
-        <v>0.72057669212289222</v>
+        <v>-0.97072534339415084</v>
       </c>
       <c r="F31">
         <f>CORREL($W$15:$Y$15,$N$15:$P$15)</f>
-        <v>0</v>
+        <v>0.75592894601845428</v>
       </c>
       <c r="G31">
         <f>CORREL($W$15:$Y$15,$Q$15:$S$15)</f>
-        <v>0.8660254037844386</v>
+        <v>0.69337524528153627</v>
       </c>
       <c r="H31">
         <f>CORREL($W$15:$Y$15,$T$15:$V$15)</f>
-        <v>0.8660254037844386</v>
+        <v>0.32732683535398877</v>
       </c>
       <c r="I31">
         <v>1</v>
@@ -3828,7 +4343,7 @@
       </c>
       <c r="K31">
         <f>CORREL($AC$15:$AE$15,$W$15:$Y$15)</f>
-        <v>0.69337524528153627</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
@@ -3837,31 +4352,31 @@
       </c>
       <c r="B32">
         <f>CORREL($Z$15:$AB$15,$B$15:$D$15)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C32">
         <f>CORREL($Z$15:$AB$15,$E$15:$G$15)</f>
-        <v>0.5</v>
+        <v>-0.27735009811261391</v>
       </c>
       <c r="D32">
         <f>CORREL($Z$15:$AB$15,$H$15:$J$15)</f>
-        <v>0.18898223650461363</v>
+        <v>-0.18898223650461363</v>
       </c>
       <c r="E32">
         <f>CORREL($Z$15:$AB$15,$K$15:$M$15)</f>
-        <v>0.96076892283052284</v>
+        <v>-0.69337524528153649</v>
       </c>
       <c r="F32">
         <f>CORREL($Z$15:$AB$15,$N$15:$P$15)</f>
-        <v>-0.8660254037844386</v>
+        <v>-0.18898223650461399</v>
       </c>
       <c r="G32">
         <f>CORREL($Z$15:$AB$15,$Q$15:$S$15)</f>
-        <v>0</v>
+        <v>-0.27735009811261474</v>
       </c>
       <c r="H32">
         <f>CORREL($Z$15:$AB$15,$Q$15:$S$15)</f>
-        <v>0</v>
+        <v>-0.27735009811261474</v>
       </c>
       <c r="I32">
         <f>CORREL($Z$15:$AB$15,$W$15:$Y$15)</f>
@@ -3872,7 +4387,7 @@
       </c>
       <c r="K32">
         <f>CORREL($AC$15:$AE$15,$Z$15:$AB$15)</f>
-        <v>-0.27735009811261452</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -3881,39 +4396,39 @@
       </c>
       <c r="B33">
         <f>CORREL($AC$15:$AE$15,$B$15:$D$15)</f>
-        <v>-0.27735009811261452</v>
+        <v>0.5</v>
       </c>
       <c r="C33">
         <f>CORREL($AC$15:$AE$15,$E$15:$G$15)</f>
-        <v>0.69337524528153627</v>
+        <v>0.97072534339415062</v>
       </c>
       <c r="D33">
         <f>CORREL($AC$15:$AE$15,$H$15:$J$15)</f>
-        <v>0.89104211121363075</v>
+        <v>0.94491118252306805</v>
       </c>
       <c r="E33">
         <f>CORREL($AC$15:$AE$15,$K$15:$M$15)</f>
-        <v>0</v>
+        <v>-0.27735009811261463</v>
       </c>
       <c r="F33">
         <f>CORREL($AC$15:$AE$15,$N$15:$P$15)</f>
-        <v>0.7205766921228921</v>
+        <v>0.94491118252306816</v>
       </c>
       <c r="G33">
         <f>CORREL($AC$15:$AE$15,$Q$15:$S$15)</f>
-        <v>0.96076892283052273</v>
+        <v>0.97072534339415084</v>
       </c>
       <c r="H33">
         <f>CORREL($AC$15:$AE$15,$Q$15:$S$15)</f>
-        <v>0.96076892283052273</v>
+        <v>0.97072534339415084</v>
       </c>
       <c r="I33">
         <f>CORREL($AC$15:$AE$15,$W$15:$Y$15)</f>
-        <v>0.69337524528153627</v>
+        <v>0.5</v>
       </c>
       <c r="J33">
         <f>CORREL($AC$15:$AE$15,$Z$15:$AB$15)</f>
-        <v>-0.27735009811261452</v>
+        <v>-0.5</v>
       </c>
       <c r="K33">
         <v>1</v>

</xml_diff>